<commit_message>
edit logo & add filtro tipo de fase
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\streamlit_tiznados\tiznados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F904637-7AEC-43EC-88D1-CCEFC69A809B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102CAAA2-01BA-4F0B-BB86-98D238CDD4B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="360">
   <si>
     <t>XY</t>
   </si>
@@ -1097,6 +1097,9 @@
   </si>
   <si>
     <t>Amistoso #1</t>
+  </si>
+  <si>
+    <t>https://youtu.be/7N6VSnEXyFQ</t>
   </si>
 </sst>
 </file>
@@ -1463,7 +1466,7 @@
   <dimension ref="A1:L96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="I3" sqref="I3:I96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1471,7 +1474,7 @@
     <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24" customWidth="1"/>
+    <col min="9" max="9" width="27.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
@@ -1537,6 +1540,9 @@
       <c r="H2" t="s">
         <v>358</v>
       </c>
+      <c r="I2" t="s">
+        <v>359</v>
+      </c>
       <c r="K2" t="s">
         <v>10</v>
       </c>
@@ -1566,6 +1572,9 @@
       <c r="H3" t="s">
         <v>358</v>
       </c>
+      <c r="I3" t="s">
+        <v>359</v>
+      </c>
       <c r="J3" t="s">
         <v>349</v>
       </c>
@@ -1601,6 +1610,9 @@
       <c r="H4" t="s">
         <v>358</v>
       </c>
+      <c r="I4" t="s">
+        <v>359</v>
+      </c>
       <c r="K4" t="s">
         <v>10</v>
       </c>
@@ -1630,6 +1642,9 @@
       <c r="H5" t="s">
         <v>358</v>
       </c>
+      <c r="I5" t="s">
+        <v>359</v>
+      </c>
       <c r="J5" t="s">
         <v>350</v>
       </c>
@@ -1665,6 +1680,9 @@
       <c r="H6" t="s">
         <v>358</v>
       </c>
+      <c r="I6" t="s">
+        <v>359</v>
+      </c>
       <c r="K6" t="s">
         <v>10</v>
       </c>
@@ -1694,6 +1712,9 @@
       <c r="H7" t="s">
         <v>358</v>
       </c>
+      <c r="I7" t="s">
+        <v>359</v>
+      </c>
       <c r="J7" t="s">
         <v>349</v>
       </c>
@@ -1726,6 +1747,9 @@
       <c r="H8" t="s">
         <v>358</v>
       </c>
+      <c r="I8" t="s">
+        <v>359</v>
+      </c>
       <c r="J8" t="s">
         <v>349</v>
       </c>
@@ -1761,6 +1785,9 @@
       <c r="H9" t="s">
         <v>358</v>
       </c>
+      <c r="I9" t="s">
+        <v>359</v>
+      </c>
       <c r="K9" t="s">
         <v>10</v>
       </c>
@@ -1787,6 +1814,9 @@
       <c r="H10" t="s">
         <v>358</v>
       </c>
+      <c r="I10" t="s">
+        <v>359</v>
+      </c>
       <c r="J10" t="s">
         <v>351</v>
       </c>
@@ -1819,6 +1849,9 @@
       <c r="H11" t="s">
         <v>358</v>
       </c>
+      <c r="I11" t="s">
+        <v>359</v>
+      </c>
       <c r="J11" t="s">
         <v>349</v>
       </c>
@@ -1854,6 +1887,9 @@
       <c r="H12" t="s">
         <v>358</v>
       </c>
+      <c r="I12" t="s">
+        <v>359</v>
+      </c>
       <c r="K12" t="s">
         <v>10</v>
       </c>
@@ -1883,6 +1919,9 @@
       <c r="H13" t="s">
         <v>358</v>
       </c>
+      <c r="I13" t="s">
+        <v>359</v>
+      </c>
       <c r="J13" t="s">
         <v>349</v>
       </c>
@@ -1912,6 +1951,9 @@
       <c r="H14" t="s">
         <v>358</v>
       </c>
+      <c r="I14" t="s">
+        <v>359</v>
+      </c>
       <c r="J14" t="s">
         <v>350</v>
       </c>
@@ -1947,6 +1989,9 @@
       <c r="H15" t="s">
         <v>358</v>
       </c>
+      <c r="I15" t="s">
+        <v>359</v>
+      </c>
       <c r="K15" t="s">
         <v>10</v>
       </c>
@@ -1976,6 +2021,9 @@
       <c r="H16" t="s">
         <v>358</v>
       </c>
+      <c r="I16" t="s">
+        <v>359</v>
+      </c>
       <c r="J16" t="s">
         <v>349</v>
       </c>
@@ -2011,6 +2059,9 @@
       <c r="H17" t="s">
         <v>358</v>
       </c>
+      <c r="I17" t="s">
+        <v>359</v>
+      </c>
       <c r="K17" t="s">
         <v>10</v>
       </c>
@@ -2040,6 +2091,9 @@
       <c r="H18" t="s">
         <v>358</v>
       </c>
+      <c r="I18" t="s">
+        <v>359</v>
+      </c>
       <c r="K18" t="s">
         <v>10</v>
       </c>
@@ -2069,6 +2123,9 @@
       <c r="H19" t="s">
         <v>358</v>
       </c>
+      <c r="I19" t="s">
+        <v>359</v>
+      </c>
       <c r="J19" t="s">
         <v>349</v>
       </c>
@@ -2104,6 +2161,9 @@
       <c r="H20" t="s">
         <v>358</v>
       </c>
+      <c r="I20" t="s">
+        <v>359</v>
+      </c>
       <c r="K20" t="s">
         <v>10</v>
       </c>
@@ -2136,6 +2196,9 @@
       <c r="H21" t="s">
         <v>358</v>
       </c>
+      <c r="I21" t="s">
+        <v>359</v>
+      </c>
       <c r="K21" t="s">
         <v>10</v>
       </c>
@@ -2165,6 +2228,9 @@
       <c r="H22" t="s">
         <v>358</v>
       </c>
+      <c r="I22" t="s">
+        <v>359</v>
+      </c>
       <c r="J22" t="s">
         <v>352</v>
       </c>
@@ -2200,6 +2266,9 @@
       <c r="H23" t="s">
         <v>358</v>
       </c>
+      <c r="I23" t="s">
+        <v>359</v>
+      </c>
       <c r="K23" t="s">
         <v>10</v>
       </c>
@@ -2229,6 +2298,9 @@
       <c r="H24" t="s">
         <v>358</v>
       </c>
+      <c r="I24" t="s">
+        <v>359</v>
+      </c>
       <c r="J24" t="s">
         <v>353</v>
       </c>
@@ -2264,6 +2336,9 @@
       <c r="H25" t="s">
         <v>358</v>
       </c>
+      <c r="I25" t="s">
+        <v>359</v>
+      </c>
       <c r="K25" t="s">
         <v>10</v>
       </c>
@@ -2293,6 +2368,9 @@
       <c r="H26" t="s">
         <v>358</v>
       </c>
+      <c r="I26" t="s">
+        <v>359</v>
+      </c>
       <c r="J26" t="s">
         <v>350</v>
       </c>
@@ -2328,6 +2406,9 @@
       <c r="H27" t="s">
         <v>358</v>
       </c>
+      <c r="I27" t="s">
+        <v>359</v>
+      </c>
       <c r="K27" t="s">
         <v>10</v>
       </c>
@@ -2357,6 +2438,9 @@
       <c r="H28" t="s">
         <v>358</v>
       </c>
+      <c r="I28" t="s">
+        <v>359</v>
+      </c>
       <c r="J28" t="s">
         <v>354</v>
       </c>
@@ -2392,6 +2476,9 @@
       <c r="H29" t="s">
         <v>358</v>
       </c>
+      <c r="I29" t="s">
+        <v>359</v>
+      </c>
       <c r="K29" t="s">
         <v>10</v>
       </c>
@@ -2424,6 +2511,9 @@
       <c r="H30" t="s">
         <v>358</v>
       </c>
+      <c r="I30" t="s">
+        <v>359</v>
+      </c>
       <c r="K30" t="s">
         <v>10</v>
       </c>
@@ -2453,6 +2543,9 @@
       <c r="H31" t="s">
         <v>358</v>
       </c>
+      <c r="I31" t="s">
+        <v>359</v>
+      </c>
       <c r="J31" t="s">
         <v>350</v>
       </c>
@@ -2488,6 +2581,9 @@
       <c r="H32" t="s">
         <v>358</v>
       </c>
+      <c r="I32" t="s">
+        <v>359</v>
+      </c>
       <c r="K32" t="s">
         <v>10</v>
       </c>
@@ -2517,6 +2613,9 @@
       <c r="H33" t="s">
         <v>358</v>
       </c>
+      <c r="I33" t="s">
+        <v>359</v>
+      </c>
       <c r="J33" t="s">
         <v>349</v>
       </c>
@@ -2552,6 +2651,9 @@
       <c r="H34" t="s">
         <v>358</v>
       </c>
+      <c r="I34" t="s">
+        <v>359</v>
+      </c>
       <c r="K34" t="s">
         <v>10</v>
       </c>
@@ -2581,6 +2683,9 @@
       <c r="H35" t="s">
         <v>358</v>
       </c>
+      <c r="I35" t="s">
+        <v>359</v>
+      </c>
       <c r="J35" t="s">
         <v>349</v>
       </c>
@@ -2616,6 +2721,9 @@
       <c r="H36" t="s">
         <v>358</v>
       </c>
+      <c r="I36" t="s">
+        <v>359</v>
+      </c>
       <c r="K36" t="s">
         <v>10</v>
       </c>
@@ -2645,6 +2753,9 @@
       <c r="H37" t="s">
         <v>358</v>
       </c>
+      <c r="I37" t="s">
+        <v>359</v>
+      </c>
       <c r="J37" t="s">
         <v>355</v>
       </c>
@@ -2680,6 +2791,9 @@
       <c r="H38" t="s">
         <v>358</v>
       </c>
+      <c r="I38" t="s">
+        <v>359</v>
+      </c>
       <c r="K38" t="s">
         <v>10</v>
       </c>
@@ -2712,6 +2826,9 @@
       <c r="H39" t="s">
         <v>358</v>
       </c>
+      <c r="I39" t="s">
+        <v>359</v>
+      </c>
       <c r="K39" t="s">
         <v>10</v>
       </c>
@@ -2744,6 +2861,9 @@
       <c r="H40" t="s">
         <v>358</v>
       </c>
+      <c r="I40" t="s">
+        <v>359</v>
+      </c>
       <c r="K40" t="s">
         <v>10</v>
       </c>
@@ -2776,6 +2896,9 @@
       <c r="H41" t="s">
         <v>358</v>
       </c>
+      <c r="I41" t="s">
+        <v>359</v>
+      </c>
       <c r="K41" t="s">
         <v>10</v>
       </c>
@@ -2808,6 +2931,9 @@
       <c r="H42" t="s">
         <v>358</v>
       </c>
+      <c r="I42" t="s">
+        <v>359</v>
+      </c>
       <c r="J42" t="s">
         <v>350</v>
       </c>
@@ -2837,6 +2963,9 @@
       <c r="H43" t="s">
         <v>358</v>
       </c>
+      <c r="I43" t="s">
+        <v>359</v>
+      </c>
       <c r="J43" t="s">
         <v>350</v>
       </c>
@@ -2872,6 +3001,9 @@
       <c r="H44" t="s">
         <v>358</v>
       </c>
+      <c r="I44" t="s">
+        <v>359</v>
+      </c>
       <c r="K44" t="s">
         <v>10</v>
       </c>
@@ -2904,6 +3036,9 @@
       <c r="H45" t="s">
         <v>358</v>
       </c>
+      <c r="I45" t="s">
+        <v>359</v>
+      </c>
       <c r="K45" t="s">
         <v>10</v>
       </c>
@@ -2933,6 +3068,9 @@
       <c r="H46" t="s">
         <v>358</v>
       </c>
+      <c r="I46" t="s">
+        <v>359</v>
+      </c>
       <c r="J46" t="s">
         <v>350</v>
       </c>
@@ -2968,6 +3106,9 @@
       <c r="H47" t="s">
         <v>358</v>
       </c>
+      <c r="I47" t="s">
+        <v>359</v>
+      </c>
       <c r="K47" t="s">
         <v>10</v>
       </c>
@@ -3000,6 +3141,9 @@
       <c r="H48" t="s">
         <v>358</v>
       </c>
+      <c r="I48" t="s">
+        <v>359</v>
+      </c>
       <c r="K48" t="s">
         <v>10</v>
       </c>
@@ -3026,6 +3170,9 @@
       <c r="H49" t="s">
         <v>358</v>
       </c>
+      <c r="I49" t="s">
+        <v>359</v>
+      </c>
       <c r="J49" t="s">
         <v>356</v>
       </c>
@@ -3058,6 +3205,9 @@
       <c r="H50" t="s">
         <v>358</v>
       </c>
+      <c r="I50" t="s">
+        <v>359</v>
+      </c>
       <c r="J50" t="s">
         <v>349</v>
       </c>
@@ -3093,6 +3243,9 @@
       <c r="H51" t="s">
         <v>358</v>
       </c>
+      <c r="I51" t="s">
+        <v>359</v>
+      </c>
       <c r="K51" t="s">
         <v>10</v>
       </c>
@@ -3125,6 +3278,9 @@
       <c r="H52" t="s">
         <v>358</v>
       </c>
+      <c r="I52" t="s">
+        <v>359</v>
+      </c>
       <c r="K52" t="s">
         <v>10</v>
       </c>
@@ -3151,6 +3307,9 @@
       <c r="H53" t="s">
         <v>358</v>
       </c>
+      <c r="I53" t="s">
+        <v>359</v>
+      </c>
       <c r="J53" t="s">
         <v>356</v>
       </c>
@@ -3186,6 +3345,9 @@
       <c r="H54" t="s">
         <v>358</v>
       </c>
+      <c r="I54" t="s">
+        <v>359</v>
+      </c>
       <c r="J54" t="s">
         <v>350</v>
       </c>
@@ -3215,6 +3377,9 @@
       <c r="H55" t="s">
         <v>358</v>
       </c>
+      <c r="I55" t="s">
+        <v>359</v>
+      </c>
       <c r="J55" t="s">
         <v>356</v>
       </c>
@@ -3247,6 +3412,9 @@
       <c r="H56" t="s">
         <v>358</v>
       </c>
+      <c r="I56" t="s">
+        <v>359</v>
+      </c>
       <c r="J56" t="s">
         <v>349</v>
       </c>
@@ -3282,6 +3450,9 @@
       <c r="H57" t="s">
         <v>358</v>
       </c>
+      <c r="I57" t="s">
+        <v>359</v>
+      </c>
       <c r="K57" t="s">
         <v>10</v>
       </c>
@@ -3311,6 +3482,9 @@
       <c r="H58" t="s">
         <v>358</v>
       </c>
+      <c r="I58" t="s">
+        <v>359</v>
+      </c>
       <c r="K58" t="s">
         <v>10</v>
       </c>
@@ -3343,6 +3517,9 @@
       <c r="H59" t="s">
         <v>358</v>
       </c>
+      <c r="I59" t="s">
+        <v>359</v>
+      </c>
       <c r="K59" t="s">
         <v>10</v>
       </c>
@@ -3372,6 +3549,9 @@
       <c r="H60" t="s">
         <v>358</v>
       </c>
+      <c r="I60" t="s">
+        <v>359</v>
+      </c>
       <c r="J60" t="s">
         <v>349</v>
       </c>
@@ -3404,6 +3584,9 @@
       <c r="H61" t="s">
         <v>358</v>
       </c>
+      <c r="I61" t="s">
+        <v>359</v>
+      </c>
       <c r="J61" t="s">
         <v>349</v>
       </c>
@@ -3439,6 +3622,9 @@
       <c r="H62" t="s">
         <v>358</v>
       </c>
+      <c r="I62" t="s">
+        <v>359</v>
+      </c>
       <c r="K62" t="s">
         <v>10</v>
       </c>
@@ -3468,6 +3654,9 @@
       <c r="H63" t="s">
         <v>358</v>
       </c>
+      <c r="I63" t="s">
+        <v>359</v>
+      </c>
       <c r="J63" t="s">
         <v>349</v>
       </c>
@@ -3503,6 +3692,9 @@
       <c r="H64" t="s">
         <v>358</v>
       </c>
+      <c r="I64" t="s">
+        <v>359</v>
+      </c>
       <c r="K64" t="s">
         <v>10</v>
       </c>
@@ -3529,6 +3721,9 @@
       <c r="H65" t="s">
         <v>358</v>
       </c>
+      <c r="I65" t="s">
+        <v>359</v>
+      </c>
       <c r="J65" t="s">
         <v>350</v>
       </c>
@@ -3561,6 +3756,9 @@
       <c r="H66" t="s">
         <v>358</v>
       </c>
+      <c r="I66" t="s">
+        <v>359</v>
+      </c>
       <c r="J66" t="s">
         <v>353</v>
       </c>
@@ -3596,6 +3794,9 @@
       <c r="H67" t="s">
         <v>358</v>
       </c>
+      <c r="I67" t="s">
+        <v>359</v>
+      </c>
       <c r="K67" t="s">
         <v>10</v>
       </c>
@@ -3628,6 +3829,9 @@
       <c r="H68" t="s">
         <v>358</v>
       </c>
+      <c r="I68" t="s">
+        <v>359</v>
+      </c>
       <c r="K68" t="s">
         <v>10</v>
       </c>
@@ -3660,6 +3864,9 @@
       <c r="H69" t="s">
         <v>358</v>
       </c>
+      <c r="I69" t="s">
+        <v>359</v>
+      </c>
       <c r="J69" t="s">
         <v>350</v>
       </c>
@@ -3689,6 +3896,9 @@
       <c r="H70" t="s">
         <v>358</v>
       </c>
+      <c r="I70" t="s">
+        <v>359</v>
+      </c>
       <c r="J70" t="s">
         <v>356</v>
       </c>
@@ -3721,6 +3931,9 @@
       <c r="H71" t="s">
         <v>358</v>
       </c>
+      <c r="I71" t="s">
+        <v>359</v>
+      </c>
       <c r="J71" t="s">
         <v>349</v>
       </c>
@@ -3756,6 +3969,9 @@
       <c r="H72" t="s">
         <v>358</v>
       </c>
+      <c r="I72" t="s">
+        <v>359</v>
+      </c>
       <c r="K72" t="s">
         <v>10</v>
       </c>
@@ -3785,6 +4001,9 @@
       <c r="H73" t="s">
         <v>358</v>
       </c>
+      <c r="I73" t="s">
+        <v>359</v>
+      </c>
       <c r="K73" t="s">
         <v>10</v>
       </c>
@@ -3817,6 +4036,9 @@
       <c r="H74" t="s">
         <v>358</v>
       </c>
+      <c r="I74" t="s">
+        <v>359</v>
+      </c>
       <c r="K74" t="s">
         <v>10</v>
       </c>
@@ -3846,6 +4068,9 @@
       <c r="H75" t="s">
         <v>358</v>
       </c>
+      <c r="I75" t="s">
+        <v>359</v>
+      </c>
       <c r="J75" t="s">
         <v>349</v>
       </c>
@@ -3875,6 +4100,9 @@
       <c r="H76" t="s">
         <v>358</v>
       </c>
+      <c r="I76" t="s">
+        <v>359</v>
+      </c>
       <c r="J76" t="s">
         <v>356</v>
       </c>
@@ -3907,6 +4135,9 @@
       <c r="H77" t="s">
         <v>358</v>
       </c>
+      <c r="I77" t="s">
+        <v>359</v>
+      </c>
       <c r="K77" t="s">
         <v>10</v>
       </c>
@@ -3939,6 +4170,9 @@
       <c r="H78" t="s">
         <v>358</v>
       </c>
+      <c r="I78" t="s">
+        <v>359</v>
+      </c>
       <c r="K78" t="s">
         <v>10</v>
       </c>
@@ -3968,6 +4202,9 @@
       <c r="H79" t="s">
         <v>358</v>
       </c>
+      <c r="I79" t="s">
+        <v>359</v>
+      </c>
       <c r="K79" t="s">
         <v>10</v>
       </c>
@@ -4000,6 +4237,9 @@
       <c r="H80" t="s">
         <v>358</v>
       </c>
+      <c r="I80" t="s">
+        <v>359</v>
+      </c>
       <c r="K80" t="s">
         <v>10</v>
       </c>
@@ -4029,6 +4269,9 @@
       <c r="H81" t="s">
         <v>358</v>
       </c>
+      <c r="I81" t="s">
+        <v>359</v>
+      </c>
       <c r="K81" t="s">
         <v>10</v>
       </c>
@@ -4061,6 +4304,9 @@
       <c r="H82" t="s">
         <v>358</v>
       </c>
+      <c r="I82" t="s">
+        <v>359</v>
+      </c>
       <c r="K82" t="s">
         <v>10</v>
       </c>
@@ -4090,6 +4336,9 @@
       <c r="H83" t="s">
         <v>358</v>
       </c>
+      <c r="I83" t="s">
+        <v>359</v>
+      </c>
       <c r="J83" t="s">
         <v>349</v>
       </c>
@@ -4125,6 +4374,9 @@
       <c r="H84" t="s">
         <v>358</v>
       </c>
+      <c r="I84" t="s">
+        <v>359</v>
+      </c>
       <c r="K84" t="s">
         <v>10</v>
       </c>
@@ -4157,6 +4409,9 @@
       <c r="H85" t="s">
         <v>358</v>
       </c>
+      <c r="I85" t="s">
+        <v>359</v>
+      </c>
       <c r="K85" t="s">
         <v>10</v>
       </c>
@@ -4186,6 +4441,9 @@
       <c r="H86" t="s">
         <v>358</v>
       </c>
+      <c r="I86" t="s">
+        <v>359</v>
+      </c>
       <c r="K86" t="s">
         <v>10</v>
       </c>
@@ -4218,6 +4476,9 @@
       <c r="H87" t="s">
         <v>358</v>
       </c>
+      <c r="I87" t="s">
+        <v>359</v>
+      </c>
       <c r="K87" t="s">
         <v>10</v>
       </c>
@@ -4250,6 +4511,9 @@
       <c r="H88" t="s">
         <v>358</v>
       </c>
+      <c r="I88" t="s">
+        <v>359</v>
+      </c>
       <c r="K88" t="s">
         <v>10</v>
       </c>
@@ -4282,6 +4546,9 @@
       <c r="H89" t="s">
         <v>358</v>
       </c>
+      <c r="I89" t="s">
+        <v>359</v>
+      </c>
       <c r="K89" t="s">
         <v>10</v>
       </c>
@@ -4314,6 +4581,9 @@
       <c r="H90" t="s">
         <v>358</v>
       </c>
+      <c r="I90" t="s">
+        <v>359</v>
+      </c>
       <c r="K90" t="s">
         <v>10</v>
       </c>
@@ -4346,6 +4616,9 @@
       <c r="H91" t="s">
         <v>358</v>
       </c>
+      <c r="I91" t="s">
+        <v>359</v>
+      </c>
       <c r="K91" t="s">
         <v>10</v>
       </c>
@@ -4378,6 +4651,9 @@
       <c r="H92" t="s">
         <v>358</v>
       </c>
+      <c r="I92" t="s">
+        <v>359</v>
+      </c>
       <c r="K92" t="s">
         <v>10</v>
       </c>
@@ -4407,6 +4683,9 @@
       <c r="H93" t="s">
         <v>358</v>
       </c>
+      <c r="I93" t="s">
+        <v>359</v>
+      </c>
       <c r="J93" t="s">
         <v>353</v>
       </c>
@@ -4442,6 +4721,9 @@
       <c r="H94" t="s">
         <v>358</v>
       </c>
+      <c r="I94" t="s">
+        <v>359</v>
+      </c>
       <c r="K94" t="s">
         <v>10</v>
       </c>
@@ -4471,6 +4753,9 @@
       <c r="H95" t="s">
         <v>358</v>
       </c>
+      <c r="I95" t="s">
+        <v>359</v>
+      </c>
       <c r="J95" t="s">
         <v>349</v>
       </c>
@@ -4487,6 +4772,9 @@
       </c>
       <c r="H96" t="s">
         <v>358</v>
+      </c>
+      <c r="I96" t="s">
+        <v>359</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrigiendo error captura de punto: mod excel output col
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\streamlit_tiznados\tiznados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102CAAA2-01BA-4F0B-BB86-98D238CDD4B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D169907C-4C7A-4B0E-A043-F2A338B96FFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1045" uniqueCount="361">
   <si>
     <t>XY</t>
   </si>
@@ -1100,6 +1100,9 @@
   </si>
   <si>
     <t>https://youtu.be/7N6VSnEXyFQ</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -1466,7 +1469,7 @@
   <dimension ref="A1:L96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:I96"/>
+      <selection activeCell="G77" sqref="G77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1811,6 +1814,9 @@
       <c r="E10" t="s">
         <v>59</v>
       </c>
+      <c r="G10" t="s">
+        <v>360</v>
+      </c>
       <c r="H10" t="s">
         <v>358</v>
       </c>
@@ -1948,6 +1954,9 @@
       <c r="E14" t="s">
         <v>76</v>
       </c>
+      <c r="G14" t="s">
+        <v>360</v>
+      </c>
       <c r="H14" t="s">
         <v>358</v>
       </c>
@@ -2960,6 +2969,9 @@
       <c r="E43" t="s">
         <v>184</v>
       </c>
+      <c r="G43" t="s">
+        <v>360</v>
+      </c>
       <c r="H43" t="s">
         <v>358</v>
       </c>
@@ -3167,6 +3179,9 @@
       <c r="E49" t="s">
         <v>207</v>
       </c>
+      <c r="G49" t="s">
+        <v>360</v>
+      </c>
       <c r="H49" t="s">
         <v>358</v>
       </c>
@@ -3304,6 +3319,9 @@
       <c r="E53" t="s">
         <v>221</v>
       </c>
+      <c r="G53" t="s">
+        <v>360</v>
+      </c>
       <c r="H53" t="s">
         <v>358</v>
       </c>
@@ -3374,6 +3392,9 @@
       <c r="E55" t="s">
         <v>228</v>
       </c>
+      <c r="G55" t="s">
+        <v>360</v>
+      </c>
       <c r="H55" t="s">
         <v>358</v>
       </c>
@@ -3718,6 +3739,9 @@
       <c r="E65" t="s">
         <v>256</v>
       </c>
+      <c r="G65" t="s">
+        <v>360</v>
+      </c>
       <c r="H65" t="s">
         <v>358</v>
       </c>
@@ -3893,6 +3917,9 @@
       <c r="E70" t="s">
         <v>271</v>
       </c>
+      <c r="G70" t="s">
+        <v>360</v>
+      </c>
       <c r="H70" t="s">
         <v>358</v>
       </c>
@@ -4096,6 +4123,9 @@
       </c>
       <c r="E76" t="s">
         <v>287</v>
+      </c>
+      <c r="G76" t="s">
+        <v>360</v>
       </c>
       <c r="H76" t="s">
         <v>358</v>

</xml_diff>

<commit_message>
corrigiendo error captura de punto:8
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\streamlit_tiznados\tiznados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D169907C-4C7A-4B0E-A043-F2A338B96FFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DF84272-FD20-4CE0-B8E3-88FFC1DCBE4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1045" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="360">
   <si>
     <t>XY</t>
   </si>
@@ -80,9 +80,6 @@
   </si>
   <si>
     <t>19:05</t>
-  </si>
-  <si>
-    <t>2T</t>
   </si>
   <si>
     <t>True</t>
@@ -1159,8 +1156,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C1975CA6-E80E-40A4-A9D5-728F867A63BD}" name="Tabla1" displayName="Tabla1" ref="A1:L96" totalsRowShown="0">
-  <autoFilter ref="A1:L96" xr:uid="{C1975CA6-E80E-40A4-A9D5-728F867A63BD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C1975CA6-E80E-40A4-A9D5-728F867A63BD}" name="Tabla1" displayName="Tabla1" ref="A1:L95" totalsRowShown="0">
+  <autoFilter ref="A1:L95" xr:uid="{C1975CA6-E80E-40A4-A9D5-728F867A63BD}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{45CCCD5A-AFCF-487D-ADA1-0BFBB6505772}" name="Fase"/>
     <tableColumn id="2" xr3:uid="{4A939A0F-B787-4665-B94F-35DE80E0B243}" name="start_time"/>
@@ -1466,10 +1463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77939FC4-FC73-4262-977F-310955BE7B1D}">
-  <dimension ref="A1:L96"/>
+  <dimension ref="A1:L95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G77" sqref="G77"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="A96" sqref="A96:XFD96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1500,7 +1497,7 @@
         <v>13</v>
       </c>
       <c r="G1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="H1" t="s">
         <v>8</v>
@@ -1509,7 +1506,7 @@
         <v>11</v>
       </c>
       <c r="J1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="K1" t="s">
         <v>9</v>
@@ -1523,69 +1520,69 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>23</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>24</v>
       </c>
-      <c r="E2" t="s">
-        <v>25</v>
-      </c>
       <c r="F2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K2" t="s">
         <v>10</v>
       </c>
       <c r="L2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
         <v>26</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>27</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>28</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>29</v>
       </c>
-      <c r="E3" t="s">
-        <v>30</v>
-      </c>
       <c r="G3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="K3" t="s">
         <v>10</v>
       </c>
       <c r="L3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -1593,69 +1590,69 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
         <v>31</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>32</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>33</v>
       </c>
-      <c r="E4" t="s">
-        <v>34</v>
-      </c>
       <c r="F4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K4" t="s">
         <v>10</v>
       </c>
       <c r="L4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
         <v>35</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>36</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>37</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>38</v>
       </c>
-      <c r="E5" t="s">
-        <v>39</v>
-      </c>
       <c r="G5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I5" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K5" t="s">
         <v>10</v>
       </c>
       <c r="L5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -1663,104 +1660,104 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s">
         <v>40</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>41</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>42</v>
-      </c>
-      <c r="E6" t="s">
-        <v>43</v>
       </c>
       <c r="F6" t="s">
         <v>6</v>
       </c>
       <c r="G6" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K6" t="s">
         <v>10</v>
       </c>
       <c r="L6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="s">
         <v>44</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>45</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>46</v>
       </c>
-      <c r="E7" t="s">
-        <v>47</v>
-      </c>
       <c r="G7" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H7" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I7" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="K7" t="s">
         <v>10</v>
       </c>
       <c r="L7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" t="s">
         <v>48</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>49</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>50</v>
       </c>
-      <c r="E8" t="s">
-        <v>51</v>
-      </c>
       <c r="G8" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H8" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I8" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J8" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="K8" t="s">
         <v>10</v>
       </c>
       <c r="L8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -1768,34 +1765,34 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" t="s">
         <v>52</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>53</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>54</v>
       </c>
-      <c r="E9" t="s">
-        <v>55</v>
-      </c>
       <c r="F9" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G9" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="H9" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I9" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K9" t="s">
         <v>10</v>
       </c>
       <c r="L9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -1803,69 +1800,69 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" t="s">
         <v>56</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>57</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>58</v>
       </c>
-      <c r="E10" t="s">
-        <v>59</v>
-      </c>
       <c r="G10" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H10" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I10" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J10" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="K10" t="s">
         <v>10</v>
       </c>
       <c r="L10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" t="s">
         <v>60</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>61</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>62</v>
       </c>
-      <c r="E11" t="s">
-        <v>63</v>
-      </c>
       <c r="G11" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H11" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I11" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J11" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="K11" t="s">
         <v>10</v>
       </c>
       <c r="L11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -1873,104 +1870,104 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" t="s">
         <v>64</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>65</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>66</v>
       </c>
-      <c r="E12" t="s">
-        <v>67</v>
-      </c>
       <c r="F12" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G12" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H12" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I12" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K12" t="s">
         <v>10</v>
       </c>
       <c r="L12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" t="s">
         <v>68</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>69</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>70</v>
       </c>
-      <c r="E13" t="s">
-        <v>71</v>
-      </c>
       <c r="G13" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H13" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I13" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J13" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="K13" t="s">
         <v>10</v>
       </c>
       <c r="L13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" t="s">
         <v>72</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>73</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>74</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>75</v>
       </c>
-      <c r="E14" t="s">
-        <v>76</v>
-      </c>
       <c r="G14" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H14" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I14" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J14" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K14" t="s">
         <v>10</v>
       </c>
       <c r="L14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -1978,69 +1975,69 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" t="s">
         <v>77</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>78</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>79</v>
-      </c>
-      <c r="E15" t="s">
-        <v>80</v>
       </c>
       <c r="F15" t="s">
         <v>6</v>
       </c>
       <c r="G15" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H15" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I15" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K15" t="s">
         <v>10</v>
       </c>
       <c r="L15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C16" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" t="s">
         <v>81</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>82</v>
       </c>
-      <c r="E16" t="s">
-        <v>83</v>
-      </c>
       <c r="G16" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H16" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I16" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J16" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="K16" t="s">
         <v>10</v>
       </c>
       <c r="L16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -2048,101 +2045,101 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" t="s">
         <v>84</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>85</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>86</v>
       </c>
-      <c r="E17" t="s">
-        <v>87</v>
-      </c>
       <c r="F17" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G17" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H17" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I17" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K17" t="s">
         <v>10</v>
       </c>
       <c r="L17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" t="s">
         <v>88</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>89</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>90</v>
       </c>
-      <c r="E18" t="s">
-        <v>91</v>
-      </c>
       <c r="G18" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H18" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I18" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K18" t="s">
         <v>10</v>
       </c>
       <c r="L18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19" t="s">
         <v>92</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>93</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>94</v>
       </c>
-      <c r="E19" t="s">
-        <v>95</v>
-      </c>
       <c r="G19" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H19" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I19" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J19" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="K19" t="s">
         <v>10</v>
       </c>
       <c r="L19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
@@ -2150,34 +2147,34 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" t="s">
         <v>96</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>97</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>98</v>
       </c>
-      <c r="E20" t="s">
-        <v>99</v>
-      </c>
       <c r="F20" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G20" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H20" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I20" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K20" t="s">
         <v>10</v>
       </c>
       <c r="L20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
@@ -2185,69 +2182,69 @@
         <v>3</v>
       </c>
       <c r="B21" t="s">
+        <v>99</v>
+      </c>
+      <c r="C21" t="s">
+        <v>99</v>
+      </c>
+      <c r="D21" t="s">
         <v>100</v>
       </c>
-      <c r="C21" t="s">
-        <v>100</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>101</v>
       </c>
-      <c r="E21" t="s">
-        <v>102</v>
-      </c>
       <c r="F21" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G21" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H21" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I21" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K21" t="s">
         <v>10</v>
       </c>
       <c r="L21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22" t="s">
+        <v>102</v>
+      </c>
+      <c r="C22" t="s">
         <v>103</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>104</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>105</v>
       </c>
-      <c r="E22" t="s">
-        <v>106</v>
-      </c>
       <c r="G22" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H22" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I22" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J22" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="K22" t="s">
         <v>10</v>
       </c>
       <c r="L22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
@@ -2255,69 +2252,69 @@
         <v>3</v>
       </c>
       <c r="B23" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23" t="s">
         <v>107</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>108</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>109</v>
       </c>
-      <c r="E23" t="s">
-        <v>110</v>
-      </c>
       <c r="F23" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G23" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H23" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I23" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K23" t="s">
         <v>10</v>
       </c>
       <c r="L23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
+        <v>110</v>
+      </c>
+      <c r="C24" t="s">
         <v>111</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>112</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>113</v>
       </c>
-      <c r="E24" t="s">
-        <v>114</v>
-      </c>
       <c r="G24" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H24" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I24" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J24" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="K24" t="s">
         <v>10</v>
       </c>
       <c r="L24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
@@ -2325,69 +2322,69 @@
         <v>3</v>
       </c>
       <c r="B25" t="s">
+        <v>114</v>
+      </c>
+      <c r="C25" t="s">
         <v>115</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>116</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>117</v>
-      </c>
-      <c r="E25" t="s">
-        <v>118</v>
       </c>
       <c r="F25" t="s">
         <v>6</v>
       </c>
       <c r="G25" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H25" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I25" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K25" t="s">
         <v>10</v>
       </c>
       <c r="L25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26" t="s">
+        <v>118</v>
+      </c>
+      <c r="C26" t="s">
         <v>119</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>120</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>121</v>
       </c>
-      <c r="E26" t="s">
-        <v>122</v>
-      </c>
       <c r="G26" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H26" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I26" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J26" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K26" t="s">
         <v>10</v>
       </c>
       <c r="L26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
@@ -2395,69 +2392,69 @@
         <v>3</v>
       </c>
       <c r="B27" t="s">
+        <v>122</v>
+      </c>
+      <c r="C27" t="s">
         <v>123</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>124</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>125</v>
       </c>
-      <c r="E27" t="s">
-        <v>126</v>
-      </c>
       <c r="F27" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G27" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H27" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I27" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K27" t="s">
         <v>10</v>
       </c>
       <c r="L27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B28" t="s">
+        <v>126</v>
+      </c>
+      <c r="C28" t="s">
         <v>127</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>128</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>129</v>
       </c>
-      <c r="E28" t="s">
-        <v>130</v>
-      </c>
       <c r="G28" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H28" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I28" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J28" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="K28" t="s">
         <v>10</v>
       </c>
       <c r="L28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
@@ -2465,34 +2462,34 @@
         <v>3</v>
       </c>
       <c r="B29" t="s">
+        <v>130</v>
+      </c>
+      <c r="C29" t="s">
         <v>131</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>132</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>133</v>
       </c>
-      <c r="E29" t="s">
-        <v>134</v>
-      </c>
       <c r="F29" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G29" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H29" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I29" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K29" t="s">
         <v>10</v>
       </c>
       <c r="L29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
@@ -2500,69 +2497,69 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
+        <v>134</v>
+      </c>
+      <c r="C30" t="s">
         <v>135</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>136</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>137</v>
       </c>
-      <c r="E30" t="s">
-        <v>138</v>
-      </c>
       <c r="F30" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G30" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H30" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I30" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K30" t="s">
         <v>10</v>
       </c>
       <c r="L30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B31" t="s">
+        <v>138</v>
+      </c>
+      <c r="C31" t="s">
         <v>139</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>140</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>141</v>
       </c>
-      <c r="E31" t="s">
-        <v>142</v>
-      </c>
       <c r="G31" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H31" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I31" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J31" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K31" t="s">
         <v>10</v>
       </c>
       <c r="L31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
@@ -2570,69 +2567,69 @@
         <v>3</v>
       </c>
       <c r="B32" t="s">
+        <v>142</v>
+      </c>
+      <c r="C32" t="s">
         <v>143</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>144</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>145</v>
       </c>
-      <c r="E32" t="s">
-        <v>146</v>
-      </c>
       <c r="F32" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G32" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H32" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I32" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K32" t="s">
         <v>10</v>
       </c>
       <c r="L32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B33" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C33" t="s">
+        <v>146</v>
+      </c>
+      <c r="D33" t="s">
         <v>147</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>148</v>
       </c>
-      <c r="E33" t="s">
-        <v>149</v>
-      </c>
       <c r="G33" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H33" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I33" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J33" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="K33" t="s">
         <v>10</v>
       </c>
       <c r="L33" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
@@ -2640,69 +2637,69 @@
         <v>3</v>
       </c>
       <c r="B34" t="s">
+        <v>149</v>
+      </c>
+      <c r="C34" t="s">
         <v>150</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>151</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>152</v>
-      </c>
-      <c r="E34" t="s">
-        <v>153</v>
       </c>
       <c r="F34" t="s">
         <v>6</v>
       </c>
       <c r="G34" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H34" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I34" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K34" t="s">
         <v>10</v>
       </c>
       <c r="L34" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B35" t="s">
+        <v>153</v>
+      </c>
+      <c r="C35" t="s">
+        <v>153</v>
+      </c>
+      <c r="D35" t="s">
         <v>154</v>
       </c>
-      <c r="C35" t="s">
-        <v>154</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>155</v>
       </c>
-      <c r="E35" t="s">
-        <v>156</v>
-      </c>
       <c r="G35" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H35" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I35" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J35" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="K35" t="s">
         <v>10</v>
       </c>
       <c r="L35" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
@@ -2710,69 +2707,69 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
+        <v>156</v>
+      </c>
+      <c r="C36" t="s">
+        <v>156</v>
+      </c>
+      <c r="D36" t="s">
         <v>157</v>
       </c>
-      <c r="C36" t="s">
-        <v>157</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>158</v>
       </c>
-      <c r="E36" t="s">
-        <v>159</v>
-      </c>
       <c r="F36" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G36" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H36" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I36" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K36" t="s">
         <v>10</v>
       </c>
       <c r="L36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B37" t="s">
+        <v>159</v>
+      </c>
+      <c r="C37" t="s">
+        <v>159</v>
+      </c>
+      <c r="D37" t="s">
         <v>160</v>
       </c>
-      <c r="C37" t="s">
-        <v>160</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>161</v>
       </c>
-      <c r="E37" t="s">
-        <v>162</v>
-      </c>
       <c r="G37" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H37" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I37" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J37" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="K37" t="s">
         <v>10</v>
       </c>
       <c r="L37" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
@@ -2780,34 +2777,34 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
+        <v>162</v>
+      </c>
+      <c r="C38" t="s">
+        <v>162</v>
+      </c>
+      <c r="D38" t="s">
         <v>163</v>
       </c>
-      <c r="C38" t="s">
-        <v>163</v>
-      </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>164</v>
-      </c>
-      <c r="E38" t="s">
-        <v>165</v>
       </c>
       <c r="F38" t="s">
         <v>2</v>
       </c>
       <c r="G38" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H38" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I38" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K38" t="s">
         <v>10</v>
       </c>
       <c r="L38" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
@@ -2815,34 +2812,34 @@
         <v>3</v>
       </c>
       <c r="B39" t="s">
+        <v>165</v>
+      </c>
+      <c r="C39" t="s">
         <v>166</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>167</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>168</v>
       </c>
-      <c r="E39" t="s">
-        <v>169</v>
-      </c>
       <c r="F39" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G39" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H39" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I39" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K39" t="s">
         <v>10</v>
       </c>
       <c r="L39" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
@@ -2850,34 +2847,34 @@
         <v>3</v>
       </c>
       <c r="B40" t="s">
+        <v>169</v>
+      </c>
+      <c r="C40" t="s">
+        <v>169</v>
+      </c>
+      <c r="D40" t="s">
         <v>170</v>
       </c>
-      <c r="C40" t="s">
-        <v>170</v>
-      </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>171</v>
-      </c>
-      <c r="E40" t="s">
-        <v>172</v>
       </c>
       <c r="F40" t="s">
         <v>6</v>
       </c>
       <c r="G40" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="H40" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I40" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K40" t="s">
         <v>10</v>
       </c>
       <c r="L40" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
@@ -2885,34 +2882,34 @@
         <v>3</v>
       </c>
       <c r="B41" t="s">
+        <v>172</v>
+      </c>
+      <c r="C41" t="s">
         <v>173</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>174</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>175</v>
       </c>
-      <c r="E41" t="s">
-        <v>176</v>
-      </c>
       <c r="F41" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G41" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H41" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I41" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K41" t="s">
         <v>10</v>
       </c>
       <c r="L41" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
@@ -2920,72 +2917,72 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
+        <v>176</v>
+      </c>
+      <c r="C42" t="s">
         <v>177</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>178</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>179</v>
       </c>
-      <c r="E42" t="s">
-        <v>180</v>
-      </c>
       <c r="F42" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G42" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H42" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I42" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J42" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K42" t="s">
         <v>10</v>
       </c>
       <c r="L42" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B43" t="s">
+        <v>180</v>
+      </c>
+      <c r="C43" t="s">
         <v>181</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>182</v>
       </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
         <v>183</v>
       </c>
-      <c r="E43" t="s">
-        <v>184</v>
-      </c>
       <c r="G43" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H43" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I43" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J43" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K43" t="s">
         <v>10</v>
       </c>
       <c r="L43" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
@@ -2993,34 +2990,34 @@
         <v>3</v>
       </c>
       <c r="B44" t="s">
+        <v>184</v>
+      </c>
+      <c r="C44" t="s">
         <v>185</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>186</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
         <v>187</v>
-      </c>
-      <c r="E44" t="s">
-        <v>188</v>
       </c>
       <c r="F44" t="s">
         <v>6</v>
       </c>
       <c r="G44" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H44" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I44" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K44" t="s">
         <v>10</v>
       </c>
       <c r="L44" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
@@ -3028,69 +3025,69 @@
         <v>3</v>
       </c>
       <c r="B45" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C45" t="s">
+        <v>188</v>
+      </c>
+      <c r="D45" t="s">
         <v>189</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
         <v>190</v>
       </c>
-      <c r="E45" t="s">
-        <v>191</v>
-      </c>
       <c r="F45" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G45" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H45" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I45" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K45" t="s">
         <v>10</v>
       </c>
       <c r="L45" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B46" t="s">
+        <v>191</v>
+      </c>
+      <c r="C46" t="s">
         <v>192</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>193</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
         <v>194</v>
       </c>
-      <c r="E46" t="s">
-        <v>195</v>
-      </c>
       <c r="G46" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H46" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I46" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J46" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K46" t="s">
         <v>10</v>
       </c>
       <c r="L46" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
@@ -3098,34 +3095,34 @@
         <v>3</v>
       </c>
       <c r="B47" t="s">
+        <v>195</v>
+      </c>
+      <c r="C47" t="s">
         <v>196</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>197</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
         <v>198</v>
       </c>
-      <c r="E47" t="s">
-        <v>199</v>
-      </c>
       <c r="F47" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G47" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H47" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I47" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K47" t="s">
         <v>10</v>
       </c>
       <c r="L47" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
@@ -3133,34 +3130,34 @@
         <v>3</v>
       </c>
       <c r="B48" t="s">
+        <v>199</v>
+      </c>
+      <c r="C48" t="s">
         <v>200</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>201</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
         <v>202</v>
       </c>
-      <c r="E48" t="s">
-        <v>203</v>
-      </c>
       <c r="F48" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G48" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H48" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I48" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K48" t="s">
         <v>10</v>
       </c>
       <c r="L48" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
@@ -3168,69 +3165,69 @@
         <v>7</v>
       </c>
       <c r="B49" t="s">
+        <v>203</v>
+      </c>
+      <c r="C49" t="s">
         <v>204</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>205</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
         <v>206</v>
       </c>
-      <c r="E49" t="s">
-        <v>207</v>
-      </c>
       <c r="G49" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H49" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I49" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J49" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="K49" t="s">
         <v>10</v>
       </c>
       <c r="L49" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B50" t="s">
+        <v>207</v>
+      </c>
+      <c r="C50" t="s">
+        <v>207</v>
+      </c>
+      <c r="D50" t="s">
         <v>208</v>
       </c>
-      <c r="C50" t="s">
-        <v>208</v>
-      </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>209</v>
       </c>
-      <c r="E50" t="s">
-        <v>210</v>
-      </c>
       <c r="G50" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H50" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I50" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J50" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="K50" t="s">
         <v>10</v>
       </c>
       <c r="L50" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
@@ -3238,34 +3235,34 @@
         <v>1</v>
       </c>
       <c r="B51" t="s">
+        <v>210</v>
+      </c>
+      <c r="C51" t="s">
+        <v>210</v>
+      </c>
+      <c r="D51" t="s">
         <v>211</v>
       </c>
-      <c r="C51" t="s">
-        <v>211</v>
-      </c>
-      <c r="D51" t="s">
+      <c r="E51" t="s">
         <v>212</v>
-      </c>
-      <c r="E51" t="s">
-        <v>213</v>
       </c>
       <c r="F51" t="s">
         <v>2</v>
       </c>
       <c r="G51" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H51" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I51" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K51" t="s">
         <v>10</v>
       </c>
       <c r="L51" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
@@ -3273,69 +3270,69 @@
         <v>3</v>
       </c>
       <c r="B52" t="s">
+        <v>213</v>
+      </c>
+      <c r="C52" t="s">
+        <v>213</v>
+      </c>
+      <c r="D52" t="s">
         <v>214</v>
       </c>
-      <c r="C52" t="s">
-        <v>214</v>
-      </c>
-      <c r="D52" t="s">
+      <c r="E52" t="s">
         <v>215</v>
       </c>
-      <c r="E52" t="s">
-        <v>216</v>
-      </c>
       <c r="F52" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G52" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H52" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I52" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K52" t="s">
         <v>10</v>
       </c>
       <c r="L52" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
+        <v>216</v>
+      </c>
+      <c r="B53" t="s">
         <v>217</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" t="s">
         <v>218</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>219</v>
       </c>
-      <c r="D53" t="s">
+      <c r="E53" t="s">
         <v>220</v>
       </c>
-      <c r="E53" t="s">
-        <v>221</v>
-      </c>
       <c r="G53" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H53" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I53" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J53" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="K53" t="s">
         <v>10</v>
       </c>
       <c r="L53" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
@@ -3343,37 +3340,37 @@
         <v>1</v>
       </c>
       <c r="B54" t="s">
+        <v>221</v>
+      </c>
+      <c r="C54" t="s">
+        <v>221</v>
+      </c>
+      <c r="D54" t="s">
         <v>222</v>
       </c>
-      <c r="C54" t="s">
-        <v>222</v>
-      </c>
-      <c r="D54" t="s">
+      <c r="E54" t="s">
         <v>223</v>
       </c>
-      <c r="E54" t="s">
-        <v>224</v>
-      </c>
       <c r="F54" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G54" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H54" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I54" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J54" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K54" t="s">
         <v>10</v>
       </c>
       <c r="L54" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
@@ -3381,69 +3378,69 @@
         <v>4</v>
       </c>
       <c r="B55" t="s">
+        <v>224</v>
+      </c>
+      <c r="C55" t="s">
         <v>225</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
         <v>226</v>
       </c>
-      <c r="D55" t="s">
+      <c r="E55" t="s">
         <v>227</v>
       </c>
-      <c r="E55" t="s">
-        <v>228</v>
-      </c>
       <c r="G55" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H55" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I55" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J55" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="K55" t="s">
         <v>10</v>
       </c>
       <c r="L55" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B56" t="s">
+        <v>228</v>
+      </c>
+      <c r="C56" t="s">
+        <v>228</v>
+      </c>
+      <c r="D56" t="s">
         <v>229</v>
       </c>
-      <c r="C56" t="s">
-        <v>229</v>
-      </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
         <v>230</v>
       </c>
-      <c r="E56" t="s">
-        <v>231</v>
-      </c>
       <c r="G56" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H56" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I56" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J56" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="K56" t="s">
         <v>10</v>
       </c>
       <c r="L56" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.2">
@@ -3451,66 +3448,66 @@
         <v>3</v>
       </c>
       <c r="B57" t="s">
+        <v>231</v>
+      </c>
+      <c r="C57" t="s">
+        <v>231</v>
+      </c>
+      <c r="D57" t="s">
         <v>232</v>
       </c>
-      <c r="C57" t="s">
-        <v>232</v>
-      </c>
-      <c r="D57" t="s">
+      <c r="E57" t="s">
         <v>233</v>
       </c>
-      <c r="E57" t="s">
-        <v>234</v>
-      </c>
       <c r="F57" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G57" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H57" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I57" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K57" t="s">
         <v>10</v>
       </c>
       <c r="L57" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B58" t="s">
+        <v>234</v>
+      </c>
+      <c r="C58" t="s">
+        <v>234</v>
+      </c>
+      <c r="D58" t="s">
         <v>235</v>
       </c>
-      <c r="C58" t="s">
-        <v>235</v>
-      </c>
-      <c r="D58" t="s">
+      <c r="E58" t="s">
         <v>236</v>
       </c>
-      <c r="E58" t="s">
-        <v>237</v>
-      </c>
       <c r="G58" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H58" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I58" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K58" t="s">
         <v>10</v>
       </c>
       <c r="L58" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
@@ -3518,104 +3515,104 @@
         <v>3</v>
       </c>
       <c r="B59" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C59" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D59" t="s">
+        <v>237</v>
+      </c>
+      <c r="E59" t="s">
         <v>238</v>
       </c>
-      <c r="E59" t="s">
-        <v>239</v>
-      </c>
       <c r="F59" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G59" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H59" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I59" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K59" t="s">
         <v>10</v>
       </c>
       <c r="L59" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B60" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C60" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D60" t="s">
+        <v>239</v>
+      </c>
+      <c r="E60" t="s">
         <v>240</v>
       </c>
-      <c r="E60" t="s">
-        <v>241</v>
-      </c>
       <c r="G60" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H60" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I60" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J60" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="K60" t="s">
         <v>10</v>
       </c>
       <c r="L60" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B61" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C61" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D61" t="s">
         <v>18</v>
       </c>
       <c r="E61" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G61" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H61" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I61" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J61" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="K61" t="s">
         <v>10</v>
       </c>
       <c r="L61" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
@@ -3623,69 +3620,69 @@
         <v>3</v>
       </c>
       <c r="B62" t="s">
+        <v>243</v>
+      </c>
+      <c r="C62" t="s">
+        <v>243</v>
+      </c>
+      <c r="D62" t="s">
         <v>244</v>
       </c>
-      <c r="C62" t="s">
-        <v>244</v>
-      </c>
-      <c r="D62" t="s">
+      <c r="E62" t="s">
         <v>245</v>
       </c>
-      <c r="E62" t="s">
-        <v>246</v>
-      </c>
       <c r="F62" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G62" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H62" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I62" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K62" t="s">
         <v>10</v>
       </c>
       <c r="L62" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B63" t="s">
+        <v>246</v>
+      </c>
+      <c r="C63" t="s">
+        <v>246</v>
+      </c>
+      <c r="D63" t="s">
         <v>247</v>
       </c>
-      <c r="C63" t="s">
-        <v>247</v>
-      </c>
-      <c r="D63" t="s">
+      <c r="E63" t="s">
         <v>248</v>
       </c>
-      <c r="E63" t="s">
-        <v>249</v>
-      </c>
       <c r="G63" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H63" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I63" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J63" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="K63" t="s">
         <v>10</v>
       </c>
       <c r="L63" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.2">
@@ -3693,34 +3690,34 @@
         <v>3</v>
       </c>
       <c r="B64" t="s">
+        <v>249</v>
+      </c>
+      <c r="C64" t="s">
+        <v>249</v>
+      </c>
+      <c r="D64" t="s">
         <v>250</v>
       </c>
-      <c r="C64" t="s">
-        <v>250</v>
-      </c>
-      <c r="D64" t="s">
+      <c r="E64" t="s">
         <v>251</v>
       </c>
-      <c r="E64" t="s">
-        <v>252</v>
-      </c>
       <c r="F64" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G64" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H64" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I64" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K64" t="s">
         <v>10</v>
       </c>
       <c r="L64" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.2">
@@ -3728,69 +3725,69 @@
         <v>4</v>
       </c>
       <c r="B65" t="s">
+        <v>252</v>
+      </c>
+      <c r="C65" t="s">
         <v>253</v>
       </c>
-      <c r="C65" t="s">
+      <c r="D65" t="s">
         <v>254</v>
       </c>
-      <c r="D65" t="s">
+      <c r="E65" t="s">
         <v>255</v>
       </c>
-      <c r="E65" t="s">
-        <v>256</v>
-      </c>
       <c r="G65" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H65" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I65" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J65" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K65" t="s">
         <v>10</v>
       </c>
       <c r="L65" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B66" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C66" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D66" t="s">
         <v>19</v>
       </c>
       <c r="E66" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G66" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H66" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I66" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J66" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="K66" t="s">
         <v>10</v>
       </c>
       <c r="L66" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.2">
@@ -3798,34 +3795,34 @@
         <v>1</v>
       </c>
       <c r="B67" t="s">
+        <v>258</v>
+      </c>
+      <c r="C67" t="s">
+        <v>258</v>
+      </c>
+      <c r="D67" t="s">
         <v>259</v>
       </c>
-      <c r="C67" t="s">
-        <v>259</v>
-      </c>
-      <c r="D67" t="s">
+      <c r="E67" t="s">
         <v>260</v>
-      </c>
-      <c r="E67" t="s">
-        <v>261</v>
       </c>
       <c r="F67" t="s">
         <v>2</v>
       </c>
       <c r="G67" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H67" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I67" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K67" t="s">
         <v>10</v>
       </c>
       <c r="L67" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.2">
@@ -3833,34 +3830,34 @@
         <v>3</v>
       </c>
       <c r="B68" t="s">
+        <v>261</v>
+      </c>
+      <c r="C68" t="s">
+        <v>261</v>
+      </c>
+      <c r="D68" t="s">
         <v>262</v>
       </c>
-      <c r="C68" t="s">
-        <v>262</v>
-      </c>
-      <c r="D68" t="s">
+      <c r="E68" t="s">
         <v>263</v>
-      </c>
-      <c r="E68" t="s">
-        <v>264</v>
       </c>
       <c r="F68" t="s">
         <v>6</v>
       </c>
       <c r="G68" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H68" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I68" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K68" t="s">
         <v>10</v>
       </c>
       <c r="L68" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.2">
@@ -3868,37 +3865,37 @@
         <v>3</v>
       </c>
       <c r="B69" t="s">
+        <v>264</v>
+      </c>
+      <c r="C69" t="s">
+        <v>264</v>
+      </c>
+      <c r="D69" t="s">
         <v>265</v>
       </c>
-      <c r="C69" t="s">
-        <v>265</v>
-      </c>
-      <c r="D69" t="s">
+      <c r="E69" t="s">
         <v>266</v>
       </c>
-      <c r="E69" t="s">
-        <v>267</v>
-      </c>
       <c r="F69" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G69" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H69" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I69" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J69" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K69" t="s">
         <v>10</v>
       </c>
       <c r="L69" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.2">
@@ -3906,69 +3903,69 @@
         <v>4</v>
       </c>
       <c r="B70" t="s">
+        <v>267</v>
+      </c>
+      <c r="C70" t="s">
         <v>268</v>
       </c>
-      <c r="C70" t="s">
+      <c r="D70" t="s">
         <v>269</v>
       </c>
-      <c r="D70" t="s">
+      <c r="E70" t="s">
         <v>270</v>
       </c>
-      <c r="E70" t="s">
-        <v>271</v>
-      </c>
       <c r="G70" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H70" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I70" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J70" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="K70" t="s">
         <v>10</v>
       </c>
       <c r="L70" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B71" t="s">
+        <v>271</v>
+      </c>
+      <c r="C71" t="s">
+        <v>271</v>
+      </c>
+      <c r="D71" t="s">
         <v>272</v>
       </c>
-      <c r="C71" t="s">
-        <v>272</v>
-      </c>
-      <c r="D71" t="s">
+      <c r="E71" t="s">
         <v>273</v>
       </c>
-      <c r="E71" t="s">
-        <v>274</v>
-      </c>
       <c r="G71" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H71" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I71" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J71" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="K71" t="s">
         <v>10</v>
       </c>
       <c r="L71" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.2">
@@ -3976,66 +3973,66 @@
         <v>3</v>
       </c>
       <c r="B72" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C72" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D72" t="s">
         <v>5</v>
       </c>
       <c r="E72" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F72" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G72" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H72" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I72" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K72" t="s">
         <v>10</v>
       </c>
       <c r="L72" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B73" t="s">
+        <v>275</v>
+      </c>
+      <c r="C73" t="s">
+        <v>275</v>
+      </c>
+      <c r="D73" t="s">
         <v>276</v>
       </c>
-      <c r="C73" t="s">
-        <v>276</v>
-      </c>
-      <c r="D73" t="s">
+      <c r="E73" t="s">
         <v>277</v>
       </c>
-      <c r="E73" t="s">
-        <v>278</v>
-      </c>
       <c r="G73" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H73" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I73" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K73" t="s">
         <v>10</v>
       </c>
       <c r="L73" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.2">
@@ -4043,69 +4040,69 @@
         <v>1</v>
       </c>
       <c r="B74" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C74" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D74" t="s">
+        <v>278</v>
+      </c>
+      <c r="E74" t="s">
         <v>279</v>
       </c>
-      <c r="E74" t="s">
-        <v>280</v>
-      </c>
       <c r="F74" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G74" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H74" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I74" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K74" t="s">
         <v>10</v>
       </c>
       <c r="L74" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B75" t="s">
+        <v>280</v>
+      </c>
+      <c r="C75" t="s">
+        <v>280</v>
+      </c>
+      <c r="D75" t="s">
         <v>281</v>
       </c>
-      <c r="C75" t="s">
-        <v>281</v>
-      </c>
-      <c r="D75" t="s">
+      <c r="E75" t="s">
         <v>282</v>
       </c>
-      <c r="E75" t="s">
-        <v>283</v>
-      </c>
       <c r="G75" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H75" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I75" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J75" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="K75" t="s">
         <v>10</v>
       </c>
       <c r="L75" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.2">
@@ -4113,66 +4110,66 @@
         <v>7</v>
       </c>
       <c r="B76" t="s">
+        <v>283</v>
+      </c>
+      <c r="C76" t="s">
         <v>284</v>
       </c>
-      <c r="C76" t="s">
+      <c r="D76" t="s">
         <v>285</v>
       </c>
-      <c r="D76" t="s">
+      <c r="E76" t="s">
         <v>286</v>
       </c>
-      <c r="E76" t="s">
-        <v>287</v>
-      </c>
       <c r="G76" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H76" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I76" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J76" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="K76" t="s">
         <v>10</v>
       </c>
       <c r="L76" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B77" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C77" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D77" t="s">
+        <v>287</v>
+      </c>
+      <c r="E77" t="s">
         <v>288</v>
       </c>
-      <c r="E77" t="s">
-        <v>289</v>
-      </c>
       <c r="G77" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H77" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I77" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K77" t="s">
         <v>10</v>
       </c>
       <c r="L77" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.2">
@@ -4180,66 +4177,66 @@
         <v>3</v>
       </c>
       <c r="B78" t="s">
+        <v>289</v>
+      </c>
+      <c r="C78" t="s">
+        <v>289</v>
+      </c>
+      <c r="D78" t="s">
         <v>290</v>
       </c>
-      <c r="C78" t="s">
-        <v>290</v>
-      </c>
-      <c r="D78" t="s">
+      <c r="E78" t="s">
         <v>291</v>
       </c>
-      <c r="E78" t="s">
-        <v>292</v>
-      </c>
       <c r="F78" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G78" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H78" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I78" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K78" t="s">
         <v>10</v>
       </c>
       <c r="L78" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B79" t="s">
+        <v>292</v>
+      </c>
+      <c r="C79" t="s">
+        <v>292</v>
+      </c>
+      <c r="D79" t="s">
         <v>293</v>
       </c>
-      <c r="C79" t="s">
-        <v>293</v>
-      </c>
-      <c r="D79" t="s">
+      <c r="E79" t="s">
         <v>294</v>
       </c>
-      <c r="E79" t="s">
-        <v>295</v>
-      </c>
       <c r="G79" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H79" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I79" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K79" t="s">
         <v>10</v>
       </c>
       <c r="L79" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.2">
@@ -4247,66 +4244,66 @@
         <v>3</v>
       </c>
       <c r="B80" t="s">
+        <v>295</v>
+      </c>
+      <c r="C80" t="s">
+        <v>295</v>
+      </c>
+      <c r="D80" t="s">
         <v>296</v>
       </c>
-      <c r="C80" t="s">
-        <v>296</v>
-      </c>
-      <c r="D80" t="s">
+      <c r="E80" t="s">
         <v>297</v>
-      </c>
-      <c r="E80" t="s">
-        <v>298</v>
       </c>
       <c r="F80" t="s">
         <v>6</v>
       </c>
       <c r="G80" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H80" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I80" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K80" t="s">
         <v>10</v>
       </c>
       <c r="L80" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B81" t="s">
+        <v>298</v>
+      </c>
+      <c r="C81" t="s">
+        <v>298</v>
+      </c>
+      <c r="D81" t="s">
         <v>299</v>
       </c>
-      <c r="C81" t="s">
-        <v>299</v>
-      </c>
-      <c r="D81" t="s">
+      <c r="E81" t="s">
         <v>300</v>
       </c>
-      <c r="E81" t="s">
-        <v>301</v>
-      </c>
       <c r="G81" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H81" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I81" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K81" t="s">
         <v>10</v>
       </c>
       <c r="L81" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.2">
@@ -4314,69 +4311,69 @@
         <v>3</v>
       </c>
       <c r="B82" t="s">
+        <v>301</v>
+      </c>
+      <c r="C82" t="s">
+        <v>301</v>
+      </c>
+      <c r="D82" t="s">
         <v>302</v>
       </c>
-      <c r="C82" t="s">
-        <v>302</v>
-      </c>
-      <c r="D82" t="s">
+      <c r="E82" t="s">
         <v>303</v>
       </c>
-      <c r="E82" t="s">
-        <v>304</v>
-      </c>
       <c r="F82" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G82" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H82" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I82" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K82" t="s">
         <v>10</v>
       </c>
       <c r="L82" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B83" t="s">
+        <v>304</v>
+      </c>
+      <c r="C83" t="s">
+        <v>304</v>
+      </c>
+      <c r="D83" t="s">
         <v>305</v>
       </c>
-      <c r="C83" t="s">
-        <v>305</v>
-      </c>
-      <c r="D83" t="s">
+      <c r="E83" t="s">
         <v>306</v>
       </c>
-      <c r="E83" t="s">
-        <v>307</v>
-      </c>
       <c r="G83" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H83" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I83" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J83" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="K83" t="s">
         <v>10</v>
       </c>
       <c r="L83" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.2">
@@ -4384,34 +4381,34 @@
         <v>1</v>
       </c>
       <c r="B84" t="s">
+        <v>307</v>
+      </c>
+      <c r="C84" t="s">
+        <v>307</v>
+      </c>
+      <c r="D84" t="s">
         <v>308</v>
       </c>
-      <c r="C84" t="s">
-        <v>308</v>
-      </c>
-      <c r="D84" t="s">
+      <c r="E84" t="s">
         <v>309</v>
       </c>
-      <c r="E84" t="s">
-        <v>310</v>
-      </c>
       <c r="F84" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G84" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H84" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I84" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K84" t="s">
         <v>10</v>
       </c>
       <c r="L84" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.2">
@@ -4419,66 +4416,66 @@
         <v>3</v>
       </c>
       <c r="B85" t="s">
+        <v>310</v>
+      </c>
+      <c r="C85" t="s">
+        <v>310</v>
+      </c>
+      <c r="D85" t="s">
         <v>311</v>
       </c>
-      <c r="C85" t="s">
-        <v>311</v>
-      </c>
-      <c r="D85" t="s">
+      <c r="E85" t="s">
         <v>312</v>
       </c>
-      <c r="E85" t="s">
-        <v>313</v>
-      </c>
       <c r="F85" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G85" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H85" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I85" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K85" t="s">
         <v>10</v>
       </c>
       <c r="L85" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B86" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C86" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D86" t="s">
+        <v>313</v>
+      </c>
+      <c r="E86" t="s">
         <v>314</v>
       </c>
-      <c r="E86" t="s">
-        <v>315</v>
-      </c>
       <c r="G86" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H86" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I86" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K86" t="s">
         <v>10</v>
       </c>
       <c r="L86" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.2">
@@ -4486,34 +4483,34 @@
         <v>1</v>
       </c>
       <c r="B87" t="s">
+        <v>315</v>
+      </c>
+      <c r="C87" t="s">
+        <v>315</v>
+      </c>
+      <c r="D87" t="s">
         <v>316</v>
       </c>
-      <c r="C87" t="s">
-        <v>316</v>
-      </c>
-      <c r="D87" t="s">
+      <c r="E87" t="s">
         <v>317</v>
-      </c>
-      <c r="E87" t="s">
-        <v>318</v>
       </c>
       <c r="F87" t="s">
         <v>2</v>
       </c>
       <c r="G87" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H87" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I87" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K87" t="s">
         <v>10</v>
       </c>
       <c r="L87" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.2">
@@ -4521,34 +4518,34 @@
         <v>3</v>
       </c>
       <c r="B88" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C88" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D88" t="s">
+        <v>318</v>
+      </c>
+      <c r="E88" t="s">
         <v>319</v>
       </c>
-      <c r="E88" t="s">
-        <v>320</v>
-      </c>
       <c r="F88" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G88" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H88" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I88" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K88" t="s">
         <v>10</v>
       </c>
       <c r="L88" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.2">
@@ -4556,34 +4553,34 @@
         <v>1</v>
       </c>
       <c r="B89" t="s">
+        <v>320</v>
+      </c>
+      <c r="C89" t="s">
+        <v>320</v>
+      </c>
+      <c r="D89" t="s">
         <v>321</v>
       </c>
-      <c r="C89" t="s">
-        <v>321</v>
-      </c>
-      <c r="D89" t="s">
+      <c r="E89" t="s">
         <v>322</v>
       </c>
-      <c r="E89" t="s">
-        <v>323</v>
-      </c>
       <c r="F89" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G89" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="H89" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I89" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K89" t="s">
         <v>10</v>
       </c>
       <c r="L89" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.2">
@@ -4591,34 +4588,34 @@
         <v>3</v>
       </c>
       <c r="B90" t="s">
+        <v>323</v>
+      </c>
+      <c r="C90" t="s">
+        <v>323</v>
+      </c>
+      <c r="D90" t="s">
         <v>324</v>
       </c>
-      <c r="C90" t="s">
-        <v>324</v>
-      </c>
-      <c r="D90" t="s">
+      <c r="E90" t="s">
         <v>325</v>
       </c>
-      <c r="E90" t="s">
-        <v>326</v>
-      </c>
       <c r="F90" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G90" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H90" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I90" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K90" t="s">
         <v>10</v>
       </c>
       <c r="L90" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.2">
@@ -4626,34 +4623,34 @@
         <v>1</v>
       </c>
       <c r="B91" t="s">
+        <v>326</v>
+      </c>
+      <c r="C91" t="s">
+        <v>326</v>
+      </c>
+      <c r="D91" t="s">
         <v>327</v>
       </c>
-      <c r="C91" t="s">
-        <v>327</v>
-      </c>
-      <c r="D91" t="s">
+      <c r="E91" t="s">
         <v>328</v>
       </c>
-      <c r="E91" t="s">
-        <v>329</v>
-      </c>
       <c r="F91" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G91" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="H91" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I91" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K91" t="s">
         <v>10</v>
       </c>
       <c r="L91" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.2">
@@ -4661,69 +4658,69 @@
         <v>3</v>
       </c>
       <c r="B92" t="s">
+        <v>329</v>
+      </c>
+      <c r="C92" t="s">
+        <v>329</v>
+      </c>
+      <c r="D92" t="s">
         <v>330</v>
       </c>
-      <c r="C92" t="s">
-        <v>330</v>
-      </c>
-      <c r="D92" t="s">
+      <c r="E92" t="s">
         <v>331</v>
       </c>
-      <c r="E92" t="s">
-        <v>332</v>
-      </c>
       <c r="F92" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G92" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H92" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I92" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K92" t="s">
         <v>10</v>
       </c>
       <c r="L92" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B93" t="s">
+        <v>332</v>
+      </c>
+      <c r="C93" t="s">
+        <v>332</v>
+      </c>
+      <c r="D93" t="s">
         <v>333</v>
       </c>
-      <c r="C93" t="s">
-        <v>333</v>
-      </c>
-      <c r="D93" t="s">
+      <c r="E93" t="s">
         <v>334</v>
       </c>
-      <c r="E93" t="s">
-        <v>335</v>
-      </c>
       <c r="G93" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H93" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I93" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J93" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="K93" t="s">
         <v>10</v>
       </c>
       <c r="L93" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.2">
@@ -4731,80 +4728,69 @@
         <v>3</v>
       </c>
       <c r="B94" t="s">
+        <v>335</v>
+      </c>
+      <c r="C94" t="s">
+        <v>335</v>
+      </c>
+      <c r="D94" t="s">
         <v>336</v>
       </c>
-      <c r="C94" t="s">
-        <v>336</v>
-      </c>
-      <c r="D94" t="s">
+      <c r="E94" t="s">
         <v>337</v>
       </c>
-      <c r="E94" t="s">
-        <v>338</v>
-      </c>
       <c r="F94" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G94" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H94" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I94" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K94" t="s">
         <v>10</v>
       </c>
       <c r="L94" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B95" t="s">
+        <v>338</v>
+      </c>
+      <c r="C95" t="s">
+        <v>338</v>
+      </c>
+      <c r="D95" t="s">
         <v>339</v>
       </c>
-      <c r="C95" t="s">
-        <v>339</v>
-      </c>
-      <c r="D95" t="s">
+      <c r="E95" t="s">
         <v>340</v>
       </c>
-      <c r="E95" t="s">
-        <v>341</v>
-      </c>
       <c r="G95" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H95" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I95" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="J95" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="K95" t="s">
         <v>10</v>
       </c>
       <c r="L95" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
-        <v>20</v>
-      </c>
-      <c r="H96" t="s">
-        <v>358</v>
-      </c>
-      <c r="I96" t="s">
-        <v>359</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add barras apiladas funcion
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\streamlit_tiznados\tiznados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCCBBE30-891B-4E22-9130-1295F615299B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A3ECC6C-B78B-491D-B0BC-72B95B39293E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1157,13 +1157,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C1975CA6-E80E-40A4-A9D5-728F867A63BD}" name="Tabla1" displayName="Tabla1" ref="A1:L95" totalsRowShown="0">
-  <autoFilter ref="A1:L95" xr:uid="{C1975CA6-E80E-40A4-A9D5-728F867A63BD}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Ataque"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:L95" xr:uid="{C1975CA6-E80E-40A4-A9D5-728F867A63BD}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{45CCCD5A-AFCF-487D-ADA1-0BFBB6505772}" name="Fase"/>
     <tableColumn id="2" xr3:uid="{4A939A0F-B787-4665-B94F-35DE80E0B243}" name="start_time"/>
@@ -1472,7 +1466,7 @@
   <dimension ref="A1:L95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="J53" sqref="J53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1556,7 +1550,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -1626,7 +1620,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -1696,7 +1690,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -1731,7 +1725,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1766,7 +1760,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1801,7 +1795,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1836,7 +1830,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1906,7 +1900,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1941,7 +1935,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>70</v>
       </c>
@@ -2011,7 +2005,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -2081,7 +2075,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -2113,7 +2107,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -2148,7 +2142,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -2218,7 +2212,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -2288,7 +2282,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -2358,7 +2352,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -2428,7 +2422,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -2498,7 +2492,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -2533,7 +2527,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -2603,7 +2597,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>24</v>
       </c>
@@ -2673,7 +2667,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>24</v>
       </c>
@@ -2708,7 +2702,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>1</v>
       </c>
@@ -2743,7 +2737,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>24</v>
       </c>
@@ -2778,7 +2772,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>1</v>
       </c>
@@ -2918,7 +2912,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>1</v>
       </c>
@@ -2956,7 +2950,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>70</v>
       </c>
@@ -3061,7 +3055,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>33</v>
       </c>
@@ -3166,7 +3160,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>7</v>
       </c>
@@ -3201,7 +3195,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>24</v>
       </c>
@@ -3236,7 +3230,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>1</v>
       </c>
@@ -3306,7 +3300,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>215</v>
       </c>
@@ -3341,7 +3335,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>1</v>
       </c>
@@ -3379,7 +3373,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>4</v>
       </c>
@@ -3414,7 +3408,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>24</v>
       </c>
@@ -3484,7 +3478,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>33</v>
       </c>
@@ -3551,7 +3545,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>33</v>
       </c>
@@ -3586,7 +3580,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>24</v>
       </c>
@@ -3656,7 +3650,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>33</v>
       </c>
@@ -3726,7 +3720,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="65" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>4</v>
       </c>
@@ -3761,7 +3755,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>24</v>
       </c>
@@ -3796,7 +3790,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="67" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>1</v>
       </c>
@@ -3904,7 +3898,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>4</v>
       </c>
@@ -3939,7 +3933,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>24</v>
       </c>
@@ -4009,7 +4003,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>33</v>
       </c>
@@ -4041,7 +4035,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="74" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>1</v>
       </c>
@@ -4076,7 +4070,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>24</v>
       </c>
@@ -4111,7 +4105,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="76" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>7</v>
       </c>
@@ -4146,7 +4140,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="77" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>33</v>
       </c>
@@ -4213,7 +4207,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="79" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>33</v>
       </c>
@@ -4280,7 +4274,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>33</v>
       </c>
@@ -4347,7 +4341,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="83" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>33</v>
       </c>
@@ -4382,7 +4376,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="84" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>1</v>
       </c>
@@ -4452,7 +4446,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="86" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>33</v>
       </c>
@@ -4484,7 +4478,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="87" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>1</v>
       </c>
@@ -4554,7 +4548,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="89" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>1</v>
       </c>
@@ -4624,7 +4618,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="91" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>1</v>
       </c>
@@ -4694,7 +4688,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="93" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>24</v>
       </c>
@@ -4764,7 +4758,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="95" spans="1:12" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
update excel add gol
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\streamlit_tiznados\tiznados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91058291-5BBF-4DB0-830F-9D942F5029B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF1A3B3-3E75-4B3D-AA74-034999F70384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1531" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1533" uniqueCount="445">
   <si>
     <t>XY</t>
   </si>
@@ -1352,6 +1352,9 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=vmWdqhzpwTA</t>
+  </si>
+  <si>
+    <t>gol</t>
   </si>
 </sst>
 </file>
@@ -1736,8 +1739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77939FC4-FC73-4262-977F-310955BE7B1D}">
   <dimension ref="A1:N134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C103" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:I130"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="K60" sqref="K60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1745,7 +1748,7 @@
     <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="43.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4000,7 +4003,7 @@
         <v>22</v>
       </c>
       <c r="G59" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="H59" t="s">
         <v>406</v>
@@ -4009,6 +4012,9 @@
         <v>443</v>
       </c>
       <c r="J59" s="1"/>
+      <c r="K59" t="s">
+        <v>444</v>
+      </c>
       <c r="L59" t="s">
         <v>9</v>
       </c>
@@ -6115,6 +6121,9 @@
         <v>443</v>
       </c>
       <c r="J114" s="1"/>
+      <c r="K114" t="s">
+        <v>444</v>
+      </c>
       <c r="L114" t="s">
         <v>420</v>
       </c>

</xml_diff>

<commit_message>
Corregir excel, add correcto a passes
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\streamlit_tiznados\tiznados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B1B3EA-FC78-40A2-8502-2B5CB029507B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41AD531D-16DA-4020-9847-52563E92FB67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5264" uniqueCount="1416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5275" uniqueCount="1416">
   <si>
     <t>XY</t>
   </si>
@@ -4274,7 +4274,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -4291,6 +4291,12 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -4316,10 +4322,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -4340,7 +4347,16 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C1975CA6-E80E-40A4-A9D5-728F867A63BD}" name="Tabla1" displayName="Tabla1" ref="A1:O430" totalsRowShown="0">
-  <autoFilter ref="A1:O430" xr:uid="{C1975CA6-E80E-40A4-A9D5-728F867A63BD}"/>
+  <autoFilter ref="A1:O430" xr:uid="{C1975CA6-E80E-40A4-A9D5-728F867A63BD}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="PASE"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="6">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{45CCCD5A-AFCF-487D-ADA1-0BFBB6505772}" name="Event"/>
     <tableColumn id="2" xr3:uid="{4A939A0F-B787-4665-B94F-35DE80E0B243}" name="start_time"/>
@@ -4652,7 +4668,7 @@
   <dimension ref="A1:O430"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L115" sqref="L115"/>
+      <selection activeCell="G402" sqref="G402"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4712,7 +4728,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>411</v>
       </c>
@@ -4743,7 +4759,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -4783,7 +4799,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -4823,7 +4839,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -4863,7 +4879,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -4903,7 +4919,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -4943,7 +4959,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -4983,7 +4999,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -5023,7 +5039,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -5063,7 +5079,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -5103,7 +5119,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -5143,7 +5159,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -5183,7 +5199,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -5223,7 +5239,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -5263,7 +5279,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -5303,7 +5319,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -5343,7 +5359,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>78</v>
       </c>
@@ -5380,7 +5396,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -5420,7 +5436,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -5460,7 +5476,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -5497,7 +5513,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -5537,7 +5553,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -5577,7 +5593,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -5617,7 +5633,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>3</v>
       </c>
@@ -5657,7 +5673,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -5697,7 +5713,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>1</v>
       </c>
@@ -5737,7 +5753,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>18</v>
       </c>
@@ -5774,7 +5790,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -5814,7 +5830,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>3</v>
       </c>
@@ -5854,7 +5870,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>3</v>
       </c>
@@ -5891,7 +5907,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>118</v>
       </c>
@@ -5928,7 +5944,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>3</v>
       </c>
@@ -5968,7 +5984,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>18</v>
       </c>
@@ -6008,7 +6024,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>3</v>
       </c>
@@ -6048,7 +6064,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>20</v>
       </c>
@@ -6088,7 +6104,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>1</v>
       </c>
@@ -6128,7 +6144,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>3</v>
       </c>
@@ -6168,7 +6184,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>18</v>
       </c>
@@ -6208,7 +6224,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>1</v>
       </c>
@@ -6248,7 +6264,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>3</v>
       </c>
@@ -6288,7 +6304,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>20</v>
       </c>
@@ -6328,7 +6344,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>3</v>
       </c>
@@ -6368,7 +6384,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>20</v>
       </c>
@@ -6408,7 +6424,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>3</v>
       </c>
@@ -6448,7 +6464,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>3</v>
       </c>
@@ -6485,7 +6501,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>3</v>
       </c>
@@ -6525,7 +6541,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>118</v>
       </c>
@@ -6562,7 +6578,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>3</v>
       </c>
@@ -6602,7 +6618,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>18</v>
       </c>
@@ -6639,7 +6655,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>18</v>
       </c>
@@ -6676,7 +6692,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>3</v>
       </c>
@@ -6716,7 +6732,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>3</v>
       </c>
@@ -6756,7 +6772,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>20</v>
       </c>
@@ -6796,7 +6812,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>1</v>
       </c>
@@ -6836,7 +6852,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>3</v>
       </c>
@@ -6876,7 +6892,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>20</v>
       </c>
@@ -6916,7 +6932,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>18</v>
       </c>
@@ -6956,7 +6972,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>78</v>
       </c>
@@ -6999,7 +7015,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>3</v>
       </c>
@@ -7039,7 +7055,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>407</v>
       </c>
@@ -7070,7 +7086,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>414</v>
       </c>
@@ -7101,7 +7117,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>78</v>
       </c>
@@ -7138,7 +7154,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>3</v>
       </c>
@@ -7178,7 +7194,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>20</v>
       </c>
@@ -7218,7 +7234,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>3</v>
       </c>
@@ -7258,7 +7274,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>3</v>
       </c>
@@ -7298,7 +7314,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>20</v>
       </c>
@@ -7338,7 +7354,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>78</v>
       </c>
@@ -7375,7 +7391,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>1</v>
       </c>
@@ -7415,7 +7431,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>20</v>
       </c>
@@ -7455,7 +7471,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>1</v>
       </c>
@@ -7495,7 +7511,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>20</v>
       </c>
@@ -7535,7 +7551,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>20</v>
       </c>
@@ -7575,7 +7591,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>3</v>
       </c>
@@ -7615,7 +7631,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>20</v>
       </c>
@@ -7655,7 +7671,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>18</v>
       </c>
@@ -7695,7 +7711,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>20</v>
       </c>
@@ -7735,7 +7751,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>1</v>
       </c>
@@ -7775,7 +7791,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>18</v>
       </c>
@@ -7815,7 +7831,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>78</v>
       </c>
@@ -7852,7 +7868,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>3</v>
       </c>
@@ -7892,7 +7908,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>3</v>
       </c>
@@ -7932,7 +7948,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>20</v>
       </c>
@@ -7972,7 +7988,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>1</v>
       </c>
@@ -8012,7 +8028,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>18</v>
       </c>
@@ -8052,7 +8068,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>78</v>
       </c>
@@ -8089,7 +8105,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>3</v>
       </c>
@@ -8129,7 +8145,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>20</v>
       </c>
@@ -8169,7 +8185,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>20</v>
       </c>
@@ -8209,7 +8225,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>1</v>
       </c>
@@ -8249,7 +8265,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>18</v>
       </c>
@@ -8289,7 +8305,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>1</v>
       </c>
@@ -8329,7 +8345,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>20</v>
       </c>
@@ -8369,7 +8385,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>3</v>
       </c>
@@ -8409,7 +8425,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>1</v>
       </c>
@@ -8449,7 +8465,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>3</v>
       </c>
@@ -8489,7 +8505,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>3</v>
       </c>
@@ -8529,7 +8545,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>18</v>
       </c>
@@ -8569,7 +8585,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>1</v>
       </c>
@@ -8609,7 +8625,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>118</v>
       </c>
@@ -8649,7 +8665,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>3</v>
       </c>
@@ -8689,7 +8705,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>20</v>
       </c>
@@ -8729,7 +8745,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>3</v>
       </c>
@@ -8769,7 +8785,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>118</v>
       </c>
@@ -8806,7 +8822,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>18</v>
       </c>
@@ -8846,7 +8862,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>78</v>
       </c>
@@ -8883,7 +8899,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>78</v>
       </c>
@@ -8920,7 +8936,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>1</v>
       </c>
@@ -8960,7 +8976,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>1</v>
       </c>
@@ -9000,7 +9016,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>18</v>
       </c>
@@ -9040,7 +9056,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>3</v>
       </c>
@@ -9080,7 +9096,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>1</v>
       </c>
@@ -9120,7 +9136,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>3</v>
       </c>
@@ -9163,7 +9179,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>18</v>
       </c>
@@ -9203,7 +9219,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>3</v>
       </c>
@@ -9243,7 +9259,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>1</v>
       </c>
@@ -9283,7 +9299,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>118</v>
       </c>
@@ -9320,7 +9336,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>18</v>
       </c>
@@ -9360,7 +9376,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>78</v>
       </c>
@@ -9397,7 +9413,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>1</v>
       </c>
@@ -9437,7 +9453,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>78</v>
       </c>
@@ -9474,7 +9490,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>1</v>
       </c>
@@ -9514,7 +9530,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>18</v>
       </c>
@@ -9554,7 +9570,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>3</v>
       </c>
@@ -9594,7 +9610,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>3</v>
       </c>
@@ -9634,7 +9650,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>422</v>
       </c>
@@ -9665,7 +9681,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>436</v>
       </c>
@@ -9706,7 +9722,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>436</v>
       </c>
@@ -9747,7 +9763,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>436</v>
       </c>
@@ -9788,7 +9804,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>436</v>
       </c>
@@ -9829,7 +9845,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>449</v>
       </c>
@@ -9864,7 +9880,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>436</v>
       </c>
@@ -9905,7 +9921,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>436</v>
       </c>
@@ -9946,7 +9962,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>460</v>
       </c>
@@ -9984,7 +10000,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>436</v>
       </c>
@@ -10025,7 +10041,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>436</v>
       </c>
@@ -10066,7 +10082,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>436</v>
       </c>
@@ -10107,7 +10123,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>436</v>
       </c>
@@ -10148,7 +10164,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>436</v>
       </c>
@@ -10189,7 +10205,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>479</v>
       </c>
@@ -10224,7 +10240,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>436</v>
       </c>
@@ -10268,7 +10284,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>436</v>
       </c>
@@ -10309,7 +10325,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>436</v>
       </c>
@@ -10350,7 +10366,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>436</v>
       </c>
@@ -10391,7 +10407,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>436</v>
       </c>
@@ -10432,7 +10448,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>436</v>
       </c>
@@ -10473,7 +10489,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>436</v>
       </c>
@@ -10511,7 +10527,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>436</v>
       </c>
@@ -10552,7 +10568,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>449</v>
       </c>
@@ -10588,7 +10604,7 @@
       </c>
     </row>
     <row r="151" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A151" t="s">
+      <c r="A151" s="3" t="s">
         <v>436</v>
       </c>
       <c r="B151" t="s">
@@ -10603,6 +10619,9 @@
       <c r="E151" t="s">
         <v>507</v>
       </c>
+      <c r="G151" s="2" t="s">
+        <v>1389</v>
+      </c>
       <c r="H151" t="s">
         <v>406</v>
       </c>
@@ -10625,7 +10644,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="152" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>436</v>
       </c>
@@ -10666,7 +10685,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="153" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>436</v>
       </c>
@@ -10707,7 +10726,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="154" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>449</v>
       </c>
@@ -10742,7 +10761,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="155" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>436</v>
       </c>
@@ -10783,7 +10802,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="156" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>436</v>
       </c>
@@ -10824,7 +10843,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="157" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>436</v>
       </c>
@@ -10865,7 +10884,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="158" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>449</v>
       </c>
@@ -10900,7 +10919,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="159" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>436</v>
       </c>
@@ -10941,7 +10960,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="160" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>436</v>
       </c>
@@ -10982,7 +11001,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="161" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>436</v>
       </c>
@@ -11023,7 +11042,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="162" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>436</v>
       </c>
@@ -11064,7 +11083,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="163" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>436</v>
       </c>
@@ -11105,7 +11124,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="164" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>436</v>
       </c>
@@ -11146,7 +11165,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="165" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>436</v>
       </c>
@@ -11187,7 +11206,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="166" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>436</v>
       </c>
@@ -11229,7 +11248,7 @@
       </c>
     </row>
     <row r="167" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A167" t="s">
+      <c r="A167" s="3" t="s">
         <v>436</v>
       </c>
       <c r="B167" t="s">
@@ -11244,6 +11263,9 @@
       <c r="E167" t="s">
         <v>559</v>
       </c>
+      <c r="G167" s="2" t="s">
+        <v>1389</v>
+      </c>
       <c r="H167" t="s">
         <v>406</v>
       </c>
@@ -11266,7 +11288,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="168" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>436</v>
       </c>
@@ -11307,7 +11329,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="169" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>436</v>
       </c>
@@ -11345,7 +11367,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="170" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>436</v>
       </c>
@@ -11389,7 +11411,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="171" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>436</v>
       </c>
@@ -11427,7 +11449,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="172" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>436</v>
       </c>
@@ -11468,7 +11490,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="173" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>436</v>
       </c>
@@ -11506,7 +11528,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="174" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>436</v>
       </c>
@@ -11547,7 +11569,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="175" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>436</v>
       </c>
@@ -11588,7 +11610,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="176" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>436</v>
       </c>
@@ -11629,7 +11651,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="177" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>436</v>
       </c>
@@ -11667,7 +11689,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="178" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>436</v>
       </c>
@@ -11708,7 +11730,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="179" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>436</v>
       </c>
@@ -11746,7 +11768,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="180" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>593</v>
       </c>
@@ -11782,7 +11804,7 @@
       </c>
     </row>
     <row r="181" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A181" t="s">
+      <c r="A181" s="3" t="s">
         <v>436</v>
       </c>
       <c r="B181" t="s">
@@ -11797,6 +11819,9 @@
       <c r="E181" t="s">
         <v>600</v>
       </c>
+      <c r="G181" s="2" t="s">
+        <v>1389</v>
+      </c>
       <c r="H181" t="s">
         <v>406</v>
       </c>
@@ -11822,7 +11847,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="182" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>436</v>
       </c>
@@ -11863,7 +11888,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="183" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>436</v>
       </c>
@@ -11904,7 +11929,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="184" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>449</v>
       </c>
@@ -11939,7 +11964,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="185" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>610</v>
       </c>
@@ -11977,7 +12002,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="186" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>610</v>
       </c>
@@ -12015,7 +12040,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="187" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>436</v>
       </c>
@@ -12056,7 +12081,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="188" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>436</v>
       </c>
@@ -12097,7 +12122,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="189" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>436</v>
       </c>
@@ -12138,7 +12163,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="190" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>436</v>
       </c>
@@ -12179,7 +12204,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="191" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>436</v>
       </c>
@@ -12220,7 +12245,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="192" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>449</v>
       </c>
@@ -12255,7 +12280,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="193" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>436</v>
       </c>
@@ -12293,7 +12318,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="194" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>436</v>
       </c>
@@ -12337,7 +12362,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="195" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>436</v>
       </c>
@@ -12378,7 +12403,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="196" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>436</v>
       </c>
@@ -12419,7 +12444,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="197" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>436</v>
       </c>
@@ -12460,7 +12485,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="198" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>436</v>
       </c>
@@ -12501,7 +12526,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="199" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>436</v>
       </c>
@@ -12542,7 +12567,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="200" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>436</v>
       </c>
@@ -12583,7 +12608,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="201" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>436</v>
       </c>
@@ -12624,7 +12649,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="202" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>593</v>
       </c>
@@ -12659,7 +12684,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="203" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>436</v>
       </c>
@@ -12700,7 +12725,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="204" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>436</v>
       </c>
@@ -12741,7 +12766,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="205" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>436</v>
       </c>
@@ -12782,7 +12807,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="206" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>436</v>
       </c>
@@ -12826,7 +12851,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="207" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>449</v>
       </c>
@@ -12861,7 +12886,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="208" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>436</v>
       </c>
@@ -12899,7 +12924,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="209" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>436</v>
       </c>
@@ -12940,7 +12965,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="210" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>436</v>
       </c>
@@ -12981,7 +13006,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="211" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>436</v>
       </c>
@@ -13022,7 +13047,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="212" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>436</v>
       </c>
@@ -13063,7 +13088,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="213" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>436</v>
       </c>
@@ -13101,7 +13126,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="214" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>436</v>
       </c>
@@ -13142,7 +13167,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="215" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>460</v>
       </c>
@@ -13181,7 +13206,7 @@
       </c>
     </row>
     <row r="216" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A216" t="s">
+      <c r="A216" s="3" t="s">
         <v>436</v>
       </c>
       <c r="B216" t="s">
@@ -13196,6 +13221,9 @@
       <c r="E216" t="s">
         <v>713</v>
       </c>
+      <c r="G216" s="2" t="s">
+        <v>1389</v>
+      </c>
       <c r="H216" t="s">
         <v>406</v>
       </c>
@@ -13218,7 +13246,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="217" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>436</v>
       </c>
@@ -13259,7 +13287,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="218" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>436</v>
       </c>
@@ -13300,7 +13328,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="219" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>436</v>
       </c>
@@ -13341,7 +13369,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="220" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>449</v>
       </c>
@@ -13376,7 +13404,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="221" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>436</v>
       </c>
@@ -13417,7 +13445,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="222" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>436</v>
       </c>
@@ -13458,7 +13486,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="223" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>436</v>
       </c>
@@ -13496,7 +13524,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="224" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>460</v>
       </c>
@@ -13534,7 +13562,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="225" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>436</v>
       </c>
@@ -13572,7 +13600,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="226" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>449</v>
       </c>
@@ -13607,7 +13635,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="227" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>460</v>
       </c>
@@ -13645,7 +13673,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="228" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>436</v>
       </c>
@@ -13686,7 +13714,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="229" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>436</v>
       </c>
@@ -13727,7 +13755,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="230" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>449</v>
       </c>
@@ -13762,7 +13790,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="231" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>436</v>
       </c>
@@ -13803,7 +13831,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="232" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>593</v>
       </c>
@@ -13838,7 +13866,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="233" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>436</v>
       </c>
@@ -13879,7 +13907,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="234" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>449</v>
       </c>
@@ -13914,7 +13942,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="235" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>436</v>
       </c>
@@ -13955,7 +13983,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="236" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>436</v>
       </c>
@@ -13996,7 +14024,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="237" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>436</v>
       </c>
@@ -14037,7 +14065,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="238" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>436</v>
       </c>
@@ -14075,7 +14103,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="239" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>436</v>
       </c>
@@ -14116,7 +14144,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="240" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>593</v>
       </c>
@@ -14151,7 +14179,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="241" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>436</v>
       </c>
@@ -14195,7 +14223,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="242" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>436</v>
       </c>
@@ -14236,7 +14264,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="243" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>436</v>
       </c>
@@ -14274,7 +14302,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="244" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>436</v>
       </c>
@@ -14315,7 +14343,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="245" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>436</v>
       </c>
@@ -14356,7 +14384,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="246" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>449</v>
       </c>
@@ -14391,7 +14419,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="247" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>436</v>
       </c>
@@ -14429,7 +14457,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="248" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>436</v>
       </c>
@@ -14470,7 +14498,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="249" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>449</v>
       </c>
@@ -14505,7 +14533,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="250" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>436</v>
       </c>
@@ -14546,7 +14574,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="251" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>436</v>
       </c>
@@ -14587,7 +14615,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="252" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>436</v>
       </c>
@@ -14628,7 +14656,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="253" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>436</v>
       </c>
@@ -14669,7 +14697,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="254" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>436</v>
       </c>
@@ -14710,7 +14738,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="255" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>436</v>
       </c>
@@ -14751,7 +14779,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="256" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>436</v>
       </c>
@@ -14792,7 +14820,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="257" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>436</v>
       </c>
@@ -14833,7 +14861,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="258" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>449</v>
       </c>
@@ -14868,7 +14896,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="259" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>436</v>
       </c>
@@ -14909,7 +14937,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="260" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>610</v>
       </c>
@@ -14947,7 +14975,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="261" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>436</v>
       </c>
@@ -14988,7 +15016,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="262" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>593</v>
       </c>
@@ -15023,7 +15051,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="263" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>460</v>
       </c>
@@ -15058,7 +15086,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="264" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>436</v>
       </c>
@@ -15099,7 +15127,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="265" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>436</v>
       </c>
@@ -15140,7 +15168,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="266" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>436</v>
       </c>
@@ -15181,7 +15209,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="267" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>436</v>
       </c>
@@ -15222,7 +15250,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="268" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>436</v>
       </c>
@@ -15263,7 +15291,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="269" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>436</v>
       </c>
@@ -15304,7 +15332,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="270" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>407</v>
       </c>
@@ -15333,7 +15361,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="271" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>886</v>
       </c>
@@ -15365,7 +15393,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="272" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>888</v>
       </c>
@@ -15397,7 +15425,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="273" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>886</v>
       </c>
@@ -15429,7 +15457,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="274" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>888</v>
       </c>
@@ -15461,7 +15489,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="275" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>414</v>
       </c>
@@ -15490,7 +15518,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="276" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>436</v>
       </c>
@@ -15531,7 +15559,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="277" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>436</v>
       </c>
@@ -15572,7 +15600,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="278" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>436</v>
       </c>
@@ -15613,7 +15641,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="279" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>436</v>
       </c>
@@ -15654,7 +15682,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="280" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>436</v>
       </c>
@@ -15695,7 +15723,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="281" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>436</v>
       </c>
@@ -15736,7 +15764,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="282" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>436</v>
       </c>
@@ -15778,7 +15806,7 @@
       </c>
     </row>
     <row r="283" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A283" t="s">
+      <c r="A283" s="3" t="s">
         <v>436</v>
       </c>
       <c r="B283" t="s">
@@ -15793,6 +15821,9 @@
       <c r="E283" t="s">
         <v>916</v>
       </c>
+      <c r="G283" s="2" t="s">
+        <v>1389</v>
+      </c>
       <c r="H283" t="s">
         <v>406</v>
       </c>
@@ -15815,7 +15846,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="284" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>436</v>
       </c>
@@ -15853,7 +15884,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="285" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>886</v>
       </c>
@@ -15885,7 +15916,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="286" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>888</v>
       </c>
@@ -15917,7 +15948,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="287" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>449</v>
       </c>
@@ -15952,7 +15983,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="288" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>886</v>
       </c>
@@ -15984,7 +16015,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="289" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>888</v>
       </c>
@@ -16016,7 +16047,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="290" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>436</v>
       </c>
@@ -16060,7 +16091,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="291" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>610</v>
       </c>
@@ -16101,7 +16132,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="292" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>593</v>
       </c>
@@ -16136,7 +16167,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="293" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>436</v>
       </c>
@@ -16174,7 +16205,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="294" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>436</v>
       </c>
@@ -16215,7 +16246,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="295" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>436</v>
       </c>
@@ -16256,7 +16287,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="296" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>436</v>
       </c>
@@ -16297,7 +16328,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="297" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>436</v>
       </c>
@@ -16338,7 +16369,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="298" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>436</v>
       </c>
@@ -16379,7 +16410,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="299" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>436</v>
       </c>
@@ -16417,7 +16448,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="300" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>436</v>
       </c>
@@ -16458,7 +16489,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="301" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>436</v>
       </c>
@@ -16499,7 +16530,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="302" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>436</v>
       </c>
@@ -16537,7 +16568,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="303" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>436</v>
       </c>
@@ -16578,7 +16609,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="304" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>436</v>
       </c>
@@ -16616,7 +16647,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="305" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>436</v>
       </c>
@@ -16657,7 +16688,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="306" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>436</v>
       </c>
@@ -16695,7 +16726,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="307" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>436</v>
       </c>
@@ -16733,7 +16764,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="308" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>436</v>
       </c>
@@ -16749,6 +16780,9 @@
       <c r="E308" t="s">
         <v>998</v>
       </c>
+      <c r="G308" t="s">
+        <v>1389</v>
+      </c>
       <c r="H308" t="s">
         <v>406</v>
       </c>
@@ -16771,7 +16805,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="309" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>436</v>
       </c>
@@ -16812,7 +16846,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="310" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>436</v>
       </c>
@@ -16853,7 +16887,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="311" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>436</v>
       </c>
@@ -16894,7 +16928,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="312" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>449</v>
       </c>
@@ -16929,7 +16963,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="313" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>436</v>
       </c>
@@ -16970,7 +17004,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="314" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>436</v>
       </c>
@@ -17008,7 +17042,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="315" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>436</v>
       </c>
@@ -17046,7 +17080,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="316" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>436</v>
       </c>
@@ -17087,7 +17121,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="317" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>436</v>
       </c>
@@ -17128,7 +17162,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="318" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>436</v>
       </c>
@@ -17169,7 +17203,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="319" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>593</v>
       </c>
@@ -17204,7 +17238,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="320" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>436</v>
       </c>
@@ -17249,7 +17283,7 @@
       </c>
     </row>
     <row r="321" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A321" t="s">
+      <c r="A321" s="3" t="s">
         <v>436</v>
       </c>
       <c r="B321" t="s">
@@ -17264,6 +17298,9 @@
       <c r="E321" t="s">
         <v>1040</v>
       </c>
+      <c r="G321" s="2" t="s">
+        <v>1389</v>
+      </c>
       <c r="H321" t="s">
         <v>406</v>
       </c>
@@ -17286,7 +17323,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="322" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>436</v>
       </c>
@@ -17327,7 +17364,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="323" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>436</v>
       </c>
@@ -17368,7 +17405,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="324" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>436</v>
       </c>
@@ -17410,7 +17447,7 @@
       </c>
     </row>
     <row r="325" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A325" t="s">
+      <c r="A325" s="3" t="s">
         <v>436</v>
       </c>
       <c r="B325" t="s">
@@ -17425,6 +17462,9 @@
       <c r="E325" t="s">
         <v>1052</v>
       </c>
+      <c r="G325" s="2" t="s">
+        <v>1389</v>
+      </c>
       <c r="H325" t="s">
         <v>406</v>
       </c>
@@ -17447,7 +17487,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="326" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
         <v>449</v>
       </c>
@@ -17482,7 +17522,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="327" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>436</v>
       </c>
@@ -17523,7 +17563,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="328" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>436</v>
       </c>
@@ -17564,7 +17604,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="329" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
         <v>436</v>
       </c>
@@ -17602,7 +17642,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="330" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
         <v>436</v>
       </c>
@@ -17643,7 +17683,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="331" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
         <v>436</v>
       </c>
@@ -17684,7 +17724,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="332" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
         <v>610</v>
       </c>
@@ -17722,7 +17762,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="333" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
         <v>436</v>
       </c>
@@ -17763,7 +17803,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="334" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
         <v>436</v>
       </c>
@@ -17801,7 +17841,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="335" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
         <v>886</v>
       </c>
@@ -17833,7 +17873,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="336" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
         <v>888</v>
       </c>
@@ -17865,7 +17905,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="337" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
         <v>436</v>
       </c>
@@ -17906,7 +17946,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="338" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
         <v>436</v>
       </c>
@@ -17947,7 +17987,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="339" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
         <v>436</v>
       </c>
@@ -17985,7 +18025,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="340" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
         <v>449</v>
       </c>
@@ -18020,7 +18060,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="341" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
         <v>436</v>
       </c>
@@ -18058,7 +18098,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="342" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
         <v>436</v>
       </c>
@@ -18099,7 +18139,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="343" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
         <v>436</v>
       </c>
@@ -18137,7 +18177,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="344" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
         <v>436</v>
       </c>
@@ -18178,7 +18218,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="345" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
         <v>436</v>
       </c>
@@ -18219,7 +18259,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="346" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
         <v>436</v>
       </c>
@@ -18257,7 +18297,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="347" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
         <v>436</v>
       </c>
@@ -18298,7 +18338,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="348" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
         <v>436</v>
       </c>
@@ -18336,7 +18376,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="349" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
         <v>460</v>
       </c>
@@ -18371,7 +18411,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="350" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
         <v>436</v>
       </c>
@@ -18412,7 +18452,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="351" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
         <v>436</v>
       </c>
@@ -18453,7 +18493,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="352" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
         <v>436</v>
       </c>
@@ -18494,7 +18534,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="353" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
         <v>449</v>
       </c>
@@ -18529,7 +18569,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="354" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A354" t="s">
         <v>436</v>
       </c>
@@ -18570,7 +18610,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="355" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A355" t="s">
         <v>436</v>
       </c>
@@ -18611,7 +18651,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="356" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A356" t="s">
         <v>449</v>
       </c>
@@ -18646,7 +18686,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="357" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A357" t="s">
         <v>436</v>
       </c>
@@ -18687,7 +18727,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="358" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A358" t="s">
         <v>460</v>
       </c>
@@ -18725,7 +18765,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="359" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
         <v>610</v>
       </c>
@@ -18766,7 +18806,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="360" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A360" t="s">
         <v>436</v>
       </c>
@@ -18807,7 +18847,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="361" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A361" t="s">
         <v>436</v>
       </c>
@@ -18848,7 +18888,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="362" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
         <v>436</v>
       </c>
@@ -18889,7 +18929,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="363" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
         <v>436</v>
       </c>
@@ -18927,7 +18967,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="364" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A364" t="s">
         <v>436</v>
       </c>
@@ -18968,7 +19008,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="365" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A365" t="s">
         <v>460</v>
       </c>
@@ -19006,7 +19046,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="366" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A366" t="s">
         <v>886</v>
       </c>
@@ -19038,7 +19078,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="367" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A367" t="s">
         <v>888</v>
       </c>
@@ -19070,7 +19110,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="368" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A368" t="s">
         <v>460</v>
       </c>
@@ -19105,7 +19145,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="369" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A369" t="s">
         <v>436</v>
       </c>
@@ -19143,7 +19183,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="370" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A370" t="s">
         <v>593</v>
       </c>
@@ -19178,7 +19218,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="371" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A371" t="s">
         <v>436</v>
       </c>
@@ -19219,7 +19259,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="372" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A372" t="s">
         <v>449</v>
       </c>
@@ -19254,7 +19294,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="373" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A373" t="s">
         <v>436</v>
       </c>
@@ -19295,7 +19335,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="374" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A374" t="s">
         <v>460</v>
       </c>
@@ -19333,7 +19373,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="375" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A375" t="s">
         <v>436</v>
       </c>
@@ -19377,7 +19417,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="376" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A376" t="s">
         <v>449</v>
       </c>
@@ -19412,7 +19452,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="377" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A377" t="s">
         <v>436</v>
       </c>
@@ -19453,7 +19493,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="378" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A378" t="s">
         <v>436</v>
       </c>
@@ -19491,7 +19531,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="379" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A379" t="s">
         <v>436</v>
       </c>
@@ -19529,7 +19569,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="380" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A380" t="s">
         <v>436</v>
       </c>
@@ -19567,7 +19607,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="381" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A381" t="s">
         <v>436</v>
       </c>
@@ -19605,7 +19645,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="382" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A382" t="s">
         <v>436</v>
       </c>
@@ -19621,6 +19661,9 @@
       <c r="E382" t="s">
         <v>1232</v>
       </c>
+      <c r="G382" t="s">
+        <v>1389</v>
+      </c>
       <c r="H382" t="s">
         <v>406</v>
       </c>
@@ -19643,7 +19686,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="383" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A383" t="s">
         <v>436</v>
       </c>
@@ -19685,7 +19728,7 @@
       </c>
     </row>
     <row r="384" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A384" t="s">
+      <c r="A384" s="3" t="s">
         <v>436</v>
       </c>
       <c r="B384" t="s">
@@ -19700,6 +19743,9 @@
       <c r="E384" t="s">
         <v>1239</v>
       </c>
+      <c r="G384" s="2" t="s">
+        <v>1389</v>
+      </c>
       <c r="H384" t="s">
         <v>406</v>
       </c>
@@ -19722,7 +19768,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="385" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A385" t="s">
         <v>436</v>
       </c>
@@ -19760,7 +19806,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="386" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A386" t="s">
         <v>436</v>
       </c>
@@ -19801,7 +19847,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="387" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A387" t="s">
         <v>436</v>
       </c>
@@ -19845,7 +19891,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="388" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A388" t="s">
         <v>436</v>
       </c>
@@ -19886,7 +19932,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="389" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A389" t="s">
         <v>436</v>
       </c>
@@ -19927,7 +19973,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="390" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A390" t="s">
         <v>436</v>
       </c>
@@ -19968,7 +20014,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="391" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A391" t="s">
         <v>436</v>
       </c>
@@ -20012,7 +20058,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="392" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A392" t="s">
         <v>610</v>
       </c>
@@ -20053,7 +20099,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="393" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A393" t="s">
         <v>436</v>
       </c>
@@ -20097,7 +20143,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="394" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A394" t="s">
         <v>449</v>
       </c>
@@ -20132,7 +20178,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="395" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A395" t="s">
         <v>436</v>
       </c>
@@ -20173,7 +20219,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="396" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A396" t="s">
         <v>436</v>
       </c>
@@ -20214,7 +20260,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="397" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A397" t="s">
         <v>436</v>
       </c>
@@ -20255,7 +20301,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="398" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A398" t="s">
         <v>436</v>
       </c>
@@ -20296,7 +20342,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="399" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A399" t="s">
         <v>593</v>
       </c>
@@ -20331,7 +20377,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="400" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A400" t="s">
         <v>436</v>
       </c>
@@ -20372,7 +20418,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="401" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A401" t="s">
         <v>460</v>
       </c>
@@ -20411,7 +20457,7 @@
       </c>
     </row>
     <row r="402" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A402" t="s">
+      <c r="A402" s="3" t="s">
         <v>436</v>
       </c>
       <c r="B402" t="s">
@@ -20426,6 +20472,9 @@
       <c r="E402" t="s">
         <v>1302</v>
       </c>
+      <c r="G402" s="2" t="s">
+        <v>1389</v>
+      </c>
       <c r="H402" t="s">
         <v>406</v>
       </c>
@@ -20451,7 +20500,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="403" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A403" t="s">
         <v>436</v>
       </c>
@@ -20492,7 +20541,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="404" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A404" t="s">
         <v>436</v>
       </c>
@@ -20533,7 +20582,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="405" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A405" t="s">
         <v>436</v>
       </c>
@@ -20574,7 +20623,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="406" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A406" t="s">
         <v>436</v>
       </c>
@@ -20618,7 +20667,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="407" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A407" t="s">
         <v>610</v>
       </c>
@@ -20656,7 +20705,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="408" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A408" t="s">
         <v>436</v>
       </c>
@@ -20697,7 +20746,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="409" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A409" t="s">
         <v>436</v>
       </c>
@@ -20735,7 +20784,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="410" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A410" t="s">
         <v>436</v>
       </c>
@@ -20779,7 +20828,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="411" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A411" t="s">
         <v>610</v>
       </c>
@@ -20820,7 +20869,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="412" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A412" t="s">
         <v>436</v>
       </c>
@@ -20861,7 +20910,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="413" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A413" t="s">
         <v>436</v>
       </c>
@@ -20902,7 +20951,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="414" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A414" t="s">
         <v>436</v>
       </c>
@@ -20940,7 +20989,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="415" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A415" t="s">
         <v>436</v>
       </c>
@@ -20981,7 +21030,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="416" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A416" t="s">
         <v>436</v>
       </c>
@@ -21019,7 +21068,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="417" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A417" t="s">
         <v>436</v>
       </c>
@@ -21060,7 +21109,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="418" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A418" t="s">
         <v>436</v>
       </c>
@@ -21101,7 +21150,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="419" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A419" t="s">
         <v>460</v>
       </c>
@@ -21139,7 +21188,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="420" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A420" t="s">
         <v>436</v>
       </c>
@@ -21180,7 +21229,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="421" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A421" t="s">
         <v>436</v>
       </c>
@@ -21221,7 +21270,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="422" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A422" t="s">
         <v>436</v>
       </c>
@@ -21259,7 +21308,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="423" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A423" t="s">
         <v>436</v>
       </c>
@@ -21300,7 +21349,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="424" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A424" t="s">
         <v>449</v>
       </c>
@@ -21335,7 +21384,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="425" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A425" t="s">
         <v>436</v>
       </c>
@@ -21373,7 +21422,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="426" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A426" t="s">
         <v>436</v>
       </c>
@@ -21411,7 +21460,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="427" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A427" t="s">
         <v>436</v>
       </c>
@@ -21452,7 +21501,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="428" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A428" t="s">
         <v>436</v>
       </c>
@@ -21493,7 +21542,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="429" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="429" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A429" t="s">
         <v>593</v>
       </c>
@@ -21528,7 +21577,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="430" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="430" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A430" t="s">
         <v>436</v>
       </c>
@@ -21879,8 +21928,9 @@
     <hyperlink ref="I430" r:id="rId305" xr:uid="{B973135E-CDAF-4C20-A4CD-E75CBE7E03A3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId306"/>
   <tableParts count="1">
-    <tablePart r:id="rId306"/>
+    <tablePart r:id="rId307"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
events excel corregir nombre player N° 5
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\streamlit_tiznados\tiznados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD3D8543-3CE5-4BFD-B2C1-80A8E776159C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8409FAE-4B46-41A9-B623-F4D7BE5D7DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5264" uniqueCount="1412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5264" uniqueCount="1413">
   <si>
     <t>XY</t>
   </si>
@@ -4256,6 +4256,9 @@
   </si>
   <si>
     <t>55;90 35;80</t>
+  </si>
+  <si>
+    <t>(5)Cassa</t>
   </si>
 </sst>
 </file>
@@ -4349,7 +4352,7 @@
   <autoFilter ref="A1:O429" xr:uid="{C1975CA6-E80E-40A4-A9D5-728F867A63BD}">
     <filterColumn colId="9">
       <filters>
-        <filter val="(22)Suparo"/>
+        <filter val="(5)Mediocentro"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -4664,7 +4667,7 @@
   <dimension ref="A1:O429"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D303" sqref="D303"/>
+      <selection activeCell="I442" sqref="I442"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10038,7 +10041,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>436</v>
       </c>
@@ -10922,7 +10925,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="159" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>436</v>
       </c>
@@ -14899,7 +14902,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="259" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>607</v>
       </c>
@@ -16571,7 +16574,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="303" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>436</v>
       </c>
@@ -17449,7 +17452,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="325" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
         <v>449</v>
       </c>
@@ -17484,7 +17487,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="326" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
         <v>436</v>
       </c>
@@ -18300,7 +18303,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="347" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
         <v>436</v>
       </c>
@@ -19040,7 +19043,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="366" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A366" t="s">
         <v>882</v>
       </c>
@@ -19060,7 +19063,7 @@
         <v>434</v>
       </c>
       <c r="J366" t="s">
-        <v>1401</v>
+        <v>1412</v>
       </c>
       <c r="M366" t="s">
         <v>420</v>
@@ -19297,7 +19300,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="373" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A373" t="s">
         <v>460</v>
       </c>
@@ -19379,7 +19382,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="375" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A375" t="s">
         <v>449</v>
       </c>
@@ -19414,7 +19417,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="376" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A376" t="s">
         <v>436</v>
       </c>
@@ -19455,7 +19458,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="377" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A377" t="s">
         <v>436</v>
       </c>
@@ -19481,7 +19484,7 @@
         <v>434</v>
       </c>
       <c r="J377" t="s">
-        <v>1401</v>
+        <v>1412</v>
       </c>
       <c r="M377" t="s">
         <v>420</v>
@@ -19730,7 +19733,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="384" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A384" t="s">
         <v>436</v>
       </c>
@@ -19756,7 +19759,7 @@
         <v>434</v>
       </c>
       <c r="J384" t="s">
-        <v>1401</v>
+        <v>1412</v>
       </c>
       <c r="M384" t="s">
         <v>420</v>
@@ -19894,7 +19897,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="388" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A388" t="s">
         <v>436</v>
       </c>
@@ -19920,7 +19923,7 @@
         <v>434</v>
       </c>
       <c r="J388" t="s">
-        <v>1401</v>
+        <v>1412</v>
       </c>
       <c r="K388" t="s">
         <v>1386</v>
@@ -20339,7 +20342,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="399" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A399" t="s">
         <v>436</v>
       </c>
@@ -20629,7 +20632,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="406" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A406" t="s">
         <v>607</v>
       </c>
@@ -20655,7 +20658,7 @@
         <v>434</v>
       </c>
       <c r="J406" t="s">
-        <v>1401</v>
+        <v>1412</v>
       </c>
       <c r="M406" t="s">
         <v>420</v>
@@ -20708,7 +20711,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="408" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A408" t="s">
         <v>436</v>
       </c>
@@ -20734,7 +20737,7 @@
         <v>434</v>
       </c>
       <c r="J408" t="s">
-        <v>1401</v>
+        <v>1412</v>
       </c>
       <c r="M408" t="s">
         <v>420</v>
@@ -20790,7 +20793,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="410" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A410" t="s">
         <v>607</v>
       </c>
@@ -20951,7 +20954,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="414" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A414" t="s">
         <v>436</v>
       </c>
@@ -20977,7 +20980,7 @@
         <v>434</v>
       </c>
       <c r="J414" t="s">
-        <v>1401</v>
+        <v>1412</v>
       </c>
       <c r="K414" t="s">
         <v>1390</v>
@@ -21030,7 +21033,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="416" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A416" t="s">
         <v>436</v>
       </c>
@@ -21056,7 +21059,7 @@
         <v>434</v>
       </c>
       <c r="J416" t="s">
-        <v>1401</v>
+        <v>1412</v>
       </c>
       <c r="K416" t="s">
         <v>1397</v>
@@ -21071,7 +21074,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="417" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A417" t="s">
         <v>436</v>
       </c>
@@ -21097,7 +21100,7 @@
         <v>434</v>
       </c>
       <c r="J417" t="s">
-        <v>1401</v>
+        <v>1412</v>
       </c>
       <c r="K417" t="s">
         <v>1399</v>
@@ -21270,7 +21273,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="422" spans="1:15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A422" t="s">
         <v>436</v>
       </c>
@@ -21296,7 +21299,7 @@
         <v>434</v>
       </c>
       <c r="J422" t="s">
-        <v>1401</v>
+        <v>1412</v>
       </c>
       <c r="K422" t="s">
         <v>1397</v>

</xml_diff>